<commit_message>
Program and table in excel run OK but need defect Trace() function
</commit_message>
<xml_diff>
--- a/DynamicPro/editDistance/editDistance.xlsx
+++ b/DynamicPro/editDistance/editDistance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoikhang/Documents/SWCPT/DynamicPro/editDistance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFC4FE8F-F73F-484B-A11F-75196C4AC9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32D0A90-7293-2146-B964-64A1064C908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>B2</t>
   </si>
@@ -84,12 +84,6 @@
     <t>Giải thuật</t>
   </si>
   <si>
-    <t>Y &lt;--</t>
-  </si>
-  <si>
-    <t>--&gt;X</t>
-  </si>
-  <si>
     <t>1. Cơ sở</t>
   </si>
   <si>
@@ -145,6 +139,12 @@
   </si>
   <si>
     <t>QABCDABEFA</t>
+  </si>
+  <si>
+    <t>X &lt;--</t>
+  </si>
+  <si>
+    <t>--&gt;Y</t>
   </si>
 </sst>
 </file>
@@ -327,7 +327,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -555,7 +585,7 @@
   <dimension ref="A1:AH18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="AE13" sqref="AE13"/>
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -590,14 +620,14 @@
       <c r="M1" s="14"/>
       <c r="N1" s="14"/>
       <c r="O1" s="13" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P1" s="12"/>
       <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="15" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
@@ -613,14 +643,14 @@
       <c r="M2" s="14"/>
       <c r="N2" s="14"/>
       <c r="O2" s="13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="P2" s="12"/>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
@@ -640,7 +670,7 @@
     </row>
     <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="13"/>
       <c r="C4" s="14"/>
@@ -672,7 +702,7 @@
     </row>
     <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="13"/>
       <c r="C5" s="14"/>
@@ -723,14 +753,14 @@
         <v>10</v>
       </c>
       <c r="AB5" s="11" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="AC5" s="1"/>
       <c r="AD5" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="AE5" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
@@ -738,10 +768,10 @@
     </row>
     <row r="6" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="14"/>
       <c r="D6" s="14"/>
@@ -763,55 +793,54 @@
         <v>0</v>
       </c>
       <c r="R6" s="2">
-        <f>R5</f>
         <v>1</v>
       </c>
       <c r="S6" s="2">
-        <f t="shared" ref="S6:AA6" si="0">S5</f>
         <v>2</v>
       </c>
       <c r="T6" s="2">
-        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="U6" s="2">
-        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="V6" s="2">
-        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="W6" s="2">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="X6" s="2">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="Y6" s="2">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="Z6" s="2">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="AA6" s="2"/>
+      <c r="AA6" s="2">
+        <v>10</v>
+      </c>
       <c r="AD6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="AE6" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="AF6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AG6" s="22" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -829,47 +858,49 @@
       <c r="P7" s="3">
         <v>1</v>
       </c>
-      <c r="Q7" s="2" cm="1">
-        <f t="array" aca="1" ref="Q7" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(Q7,-1,-1),MIN(1+OFFSET(Q7,0,-1),1+OFFSET(Q7,-1,0),1+OFFSET(Q7,-1,-1)))</f>
+      <c r="Q7" s="2">
         <v>1</v>
       </c>
       <c r="R7" s="2" cm="1">
-        <f t="array" aca="1" ref="R7" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(R7,-1,-1),MIN(1+OFFSET(R7,0,-1),1+OFFSET(R7,-1,0),1+OFFSET(R7,-1,-1)))</f>
+        <f t="array" aca="1" ref="R7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,R$5+1,1),OFFSET(R7,-1,-1),MIN(1+OFFSET(R7,0,-1),1+OFFSET(R7,-1,0),1+OFFSET(R7,-1,-1)))</f>
         <v>1</v>
       </c>
       <c r="S7" s="2" cm="1">
-        <f t="array" aca="1" ref="S7" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(S7,-1,-1),MIN(1+OFFSET(S7,0,-1),1+OFFSET(S7,-1,0),1+OFFSET(S7,-1,-1)))</f>
+        <f t="array" aca="1" ref="S7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,S$5+1,1),OFFSET(S7,-1,-1),MIN(1+OFFSET(S7,0,-1),1+OFFSET(S7,-1,0),1+OFFSET(S7,-1,-1)))</f>
         <v>2</v>
       </c>
       <c r="T7" s="2" cm="1">
-        <f t="array" aca="1" ref="T7" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(T7,-1,-1),MIN(1+OFFSET(T7,0,-1),1+OFFSET(T7,-1,0),1+OFFSET(T7,-1,-1)))</f>
+        <f t="array" aca="1" ref="T7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,T$5+1,1),OFFSET(T7,-1,-1),MIN(1+OFFSET(T7,0,-1),1+OFFSET(T7,-1,0),1+OFFSET(T7,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="U7" s="2" cm="1">
-        <f t="array" aca="1" ref="U7" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(U7,-1,-1),MIN(1+OFFSET(U7,0,-1),1+OFFSET(U7,-1,0),1+OFFSET(U7,-1,-1)))</f>
+        <f t="array" aca="1" ref="U7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,U$5+1,1),OFFSET(U7,-1,-1),MIN(1+OFFSET(U7,0,-1),1+OFFSET(U7,-1,0),1+OFFSET(U7,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="V7" s="2" cm="1">
-        <f t="array" aca="1" ref="V7" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(V7,-1,-1),MIN(1+OFFSET(V7,0,-1),1+OFFSET(V7,-1,0),1+OFFSET(V7,-1,-1)))</f>
+        <f t="array" aca="1" ref="V7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,V$5+1,1),OFFSET(V7,-1,-1),MIN(1+OFFSET(V7,0,-1),1+OFFSET(V7,-1,0),1+OFFSET(V7,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="W7" s="2" cm="1">
-        <f t="array" aca="1" ref="W7" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(W7,-1,-1),MIN(1+OFFSET(W7,0,-1),1+OFFSET(W7,-1,0),1+OFFSET(W7,-1,-1)))</f>
+        <f t="array" aca="1" ref="W7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,W$5+1,1),OFFSET(W7,-1,-1),MIN(1+OFFSET(W7,0,-1),1+OFFSET(W7,-1,0),1+OFFSET(W7,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="X7" s="2" cm="1">
-        <f t="array" aca="1" ref="X7" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(X7,-1,-1),MIN(1+OFFSET(X7,0,-1),1+OFFSET(X7,-1,0),1+OFFSET(X7,-1,-1)))</f>
+        <f t="array" aca="1" ref="X7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,X$5+1,1),OFFSET(X7,-1,-1),MIN(1+OFFSET(X7,0,-1),1+OFFSET(X7,-1,0),1+OFFSET(X7,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="Y7" s="2" cm="1">
-        <f t="array" aca="1" ref="Y7" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(Y7,-1,-1),MIN(1+OFFSET(Y7,0,-1),1+OFFSET(Y7,-1,0),1+OFFSET(Y7,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y7,-1,-1),MIN(1+OFFSET(Y7,0,-1),1+OFFSET(Y7,-1,0),1+OFFSET(Y7,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="Z7" s="2" cm="1">
-        <f t="array" aca="1" ref="Z7" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P7+1,1),OFFSET(Z7,-1,-1),MIN(1+OFFSET(Z7,0,-1),1+OFFSET(Z7,-1,0),1+OFFSET(Z7,-1,-1)))</f>
+        <f t="array" aca="1" ref="Z7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z7,-1,-1),MIN(1+OFFSET(Z7,0,-1),1+OFFSET(Z7,-1,0),1+OFFSET(Z7,-1,-1)))</f>
         <v>9</v>
       </c>
-      <c r="AA7" s="2"/>
+      <c r="AA7" s="2" cm="1">
+        <f t="array" aca="1" ref="AA7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA7,-1,-1),MIN(1+OFFSET(AA7,0,-1),1+OFFSET(AA7,-1,0),1+OFFSET(AA7,-1,-1)))</f>
+        <v>10</v>
+      </c>
       <c r="AB7" s="1"/>
       <c r="AC7" s="1"/>
       <c r="AD7" s="7" t="str">
@@ -886,10 +917,10 @@
     </row>
     <row r="8" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="17" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14"/>
@@ -907,55 +938,57 @@
       <c r="P8" s="3">
         <v>2</v>
       </c>
-      <c r="Q8" s="2" cm="1">
-        <f t="array" aca="1" ref="Q8" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(Q8,-1,-1),MIN(1+OFFSET(Q8,0,-1),1+OFFSET(Q8,-1,0),1+OFFSET(Q8,-1,-1)))</f>
+      <c r="Q8" s="2">
         <v>2</v>
       </c>
       <c r="R8" s="2" cm="1">
-        <f t="array" aca="1" ref="R8" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(R8,-1,-1),MIN(1+OFFSET(R8,0,-1),1+OFFSET(R8,-1,0),1+OFFSET(R8,-1,-1)))</f>
+        <f t="array" aca="1" ref="R8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,R$5+1,1),OFFSET(R8,-1,-1),MIN(1+OFFSET(R8,0,-1),1+OFFSET(R8,-1,0),1+OFFSET(R8,-1,-1)))</f>
         <v>2</v>
       </c>
       <c r="S8" s="2" cm="1">
-        <f t="array" aca="1" ref="S8" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(S8,-1,-1),MIN(1+OFFSET(S8,0,-1),1+OFFSET(S8,-1,0),1+OFFSET(S8,-1,-1)))</f>
+        <f t="array" aca="1" ref="S8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,S$5+1,1),OFFSET(S8,-1,-1),MIN(1+OFFSET(S8,0,-1),1+OFFSET(S8,-1,0),1+OFFSET(S8,-1,-1)))</f>
         <v>2</v>
       </c>
       <c r="T8" s="2" cm="1">
-        <f t="array" aca="1" ref="T8" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(T8,-1,-1),MIN(1+OFFSET(T8,0,-1),1+OFFSET(T8,-1,0),1+OFFSET(T8,-1,-1)))</f>
+        <f t="array" aca="1" ref="T8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,T$5+1,1),OFFSET(T8,-1,-1),MIN(1+OFFSET(T8,0,-1),1+OFFSET(T8,-1,0),1+OFFSET(T8,-1,-1)))</f>
+        <v>2</v>
+      </c>
+      <c r="U8" s="2" cm="1">
+        <f t="array" aca="1" ref="U8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,U$5+1,1),OFFSET(U8,-1,-1),MIN(1+OFFSET(U8,0,-1),1+OFFSET(U8,-1,0),1+OFFSET(U8,-1,-1)))</f>
         <v>3</v>
       </c>
-      <c r="U8" s="2" cm="1">
-        <f t="array" aca="1" ref="U8" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(U8,-1,-1),MIN(1+OFFSET(U8,0,-1),1+OFFSET(U8,-1,0),1+OFFSET(U8,-1,-1)))</f>
+      <c r="V8" s="2" cm="1">
+        <f t="array" aca="1" ref="V8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,V$5+1,1),OFFSET(V8,-1,-1),MIN(1+OFFSET(V8,0,-1),1+OFFSET(V8,-1,0),1+OFFSET(V8,-1,-1)))</f>
         <v>4</v>
       </c>
-      <c r="V8" s="2" cm="1">
-        <f t="array" aca="1" ref="V8" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(V8,-1,-1),MIN(1+OFFSET(V8,0,-1),1+OFFSET(V8,-1,0),1+OFFSET(V8,-1,-1)))</f>
-        <v>5</v>
-      </c>
       <c r="W8" s="2" cm="1">
-        <f t="array" aca="1" ref="W8" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(W8,-1,-1),MIN(1+OFFSET(W8,0,-1),1+OFFSET(W8,-1,0),1+OFFSET(W8,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="W8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,W$5+1,1),OFFSET(W8,-1,-1),MIN(1+OFFSET(W8,0,-1),1+OFFSET(W8,-1,0),1+OFFSET(W8,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="X8" s="2" cm="1">
-        <f t="array" aca="1" ref="X8" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(X8,-1,-1),MIN(1+OFFSET(X8,0,-1),1+OFFSET(X8,-1,0),1+OFFSET(X8,-1,-1)))</f>
+        <f t="array" aca="1" ref="X8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,X$5+1,1),OFFSET(X8,-1,-1),MIN(1+OFFSET(X8,0,-1),1+OFFSET(X8,-1,0),1+OFFSET(X8,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="Y8" s="2" cm="1">
-        <f t="array" aca="1" ref="Y8" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(Y8,-1,-1),MIN(1+OFFSET(Y8,0,-1),1+OFFSET(Y8,-1,0),1+OFFSET(Y8,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y8,-1,-1),MIN(1+OFFSET(Y8,0,-1),1+OFFSET(Y8,-1,0),1+OFFSET(Y8,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="Z8" s="2" cm="1">
-        <f t="array" aca="1" ref="Z8" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P8+1,1),OFFSET(Z8,-1,-1),MIN(1+OFFSET(Z8,0,-1),1+OFFSET(Z8,-1,0),1+OFFSET(Z8,-1,-1)))</f>
+        <f t="array" aca="1" ref="Z8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z8,-1,-1),MIN(1+OFFSET(Z8,0,-1),1+OFFSET(Z8,-1,0),1+OFFSET(Z8,-1,-1)))</f>
         <v>8</v>
       </c>
-      <c r="AA8" s="2"/>
+      <c r="AA8" s="2" cm="1">
+        <f t="array" aca="1" ref="AA8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA8,-1,-1),MIN(1+OFFSET(AA8,0,-1),1+OFFSET(AA8,-1,0),1+OFFSET(AA8,-1,-1)))</f>
+        <v>9</v>
+      </c>
       <c r="AB8" s="1"/>
       <c r="AC8" s="1"/>
       <c r="AD8" s="7" t="str">
-        <f t="shared" ref="AD8:AE16" si="1">MID(AD$6,$P8,1)</f>
+        <f t="shared" ref="AD8:AE16" si="0">MID(AD$6,$P8,1)</f>
         <v>B</v>
       </c>
       <c r="AE8" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="AF8" s="1"/>
@@ -964,10 +997,10 @@
     </row>
     <row r="9" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="14"/>
@@ -985,55 +1018,57 @@
       <c r="P9" s="3">
         <v>3</v>
       </c>
-      <c r="Q9" s="2" cm="1">
-        <f t="array" aca="1" ref="Q9" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(Q9,-1,-1),MIN(1+OFFSET(Q9,0,-1),1+OFFSET(Q9,-1,0),1+OFFSET(Q9,-1,-1)))</f>
+      <c r="Q9" s="2">
         <v>3</v>
       </c>
       <c r="R9" s="2" cm="1">
-        <f t="array" aca="1" ref="R9" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(R9,-1,-1),MIN(1+OFFSET(R9,0,-1),1+OFFSET(R9,-1,0),1+OFFSET(R9,-1,-1)))</f>
+        <f t="array" aca="1" ref="R9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,R$5+1,1),OFFSET(R9,-1,-1),MIN(1+OFFSET(R9,0,-1),1+OFFSET(R9,-1,0),1+OFFSET(R9,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="S9" s="2" cm="1">
-        <f t="array" aca="1" ref="S9" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(S9,-1,-1),MIN(1+OFFSET(S9,0,-1),1+OFFSET(S9,-1,0),1+OFFSET(S9,-1,-1)))</f>
+        <f t="array" aca="1" ref="S9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,S$5+1,1),OFFSET(S9,-1,-1),MIN(1+OFFSET(S9,0,-1),1+OFFSET(S9,-1,0),1+OFFSET(S9,-1,-1)))</f>
+        <v>3</v>
+      </c>
+      <c r="T9" s="2" cm="1">
+        <f t="array" aca="1" ref="T9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,T$5+1,1),OFFSET(T9,-1,-1),MIN(1+OFFSET(T9,0,-1),1+OFFSET(T9,-1,0),1+OFFSET(T9,-1,-1)))</f>
         <v>2</v>
       </c>
-      <c r="T9" s="2" cm="1">
-        <f t="array" aca="1" ref="T9" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(T9,-1,-1),MIN(1+OFFSET(T9,0,-1),1+OFFSET(T9,-1,0),1+OFFSET(T9,-1,-1)))</f>
-        <v>2</v>
-      </c>
       <c r="U9" s="2" cm="1">
-        <f t="array" aca="1" ref="U9" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(U9,-1,-1),MIN(1+OFFSET(U9,0,-1),1+OFFSET(U9,-1,0),1+OFFSET(U9,-1,-1)))</f>
+        <f t="array" aca="1" ref="U9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,U$5+1,1),OFFSET(U9,-1,-1),MIN(1+OFFSET(U9,0,-1),1+OFFSET(U9,-1,0),1+OFFSET(U9,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="V9" s="2" cm="1">
-        <f t="array" aca="1" ref="V9" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(V9,-1,-1),MIN(1+OFFSET(V9,0,-1),1+OFFSET(V9,-1,0),1+OFFSET(V9,-1,-1)))</f>
+        <f t="array" aca="1" ref="V9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,V$5+1,1),OFFSET(V9,-1,-1),MIN(1+OFFSET(V9,0,-1),1+OFFSET(V9,-1,0),1+OFFSET(V9,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="W9" s="2" cm="1">
-        <f t="array" aca="1" ref="W9" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(W9,-1,-1),MIN(1+OFFSET(W9,0,-1),1+OFFSET(W9,-1,0),1+OFFSET(W9,-1,-1)))</f>
+        <f t="array" aca="1" ref="W9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,W$5+1,1),OFFSET(W9,-1,-1),MIN(1+OFFSET(W9,0,-1),1+OFFSET(W9,-1,0),1+OFFSET(W9,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="X9" s="2" cm="1">
-        <f t="array" aca="1" ref="X9" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(X9,-1,-1),MIN(1+OFFSET(X9,0,-1),1+OFFSET(X9,-1,0),1+OFFSET(X9,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="X9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,X$5+1,1),OFFSET(X9,-1,-1),MIN(1+OFFSET(X9,0,-1),1+OFFSET(X9,-1,0),1+OFFSET(X9,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="Y9" s="2" cm="1">
-        <f t="array" aca="1" ref="Y9" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(Y9,-1,-1),MIN(1+OFFSET(Y9,0,-1),1+OFFSET(Y9,-1,0),1+OFFSET(Y9,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="Y9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y9,-1,-1),MIN(1+OFFSET(Y9,0,-1),1+OFFSET(Y9,-1,0),1+OFFSET(Y9,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="Z9" s="2" cm="1">
-        <f t="array" aca="1" ref="Z9" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P9+1,1),OFFSET(Z9,-1,-1),MIN(1+OFFSET(Z9,0,-1),1+OFFSET(Z9,-1,0),1+OFFSET(Z9,-1,-1)))</f>
+        <f t="array" aca="1" ref="Z9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z9,-1,-1),MIN(1+OFFSET(Z9,0,-1),1+OFFSET(Z9,-1,0),1+OFFSET(Z9,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="AA9" s="2" cm="1">
+        <f t="array" aca="1" ref="AA9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA9,-1,-1),MIN(1+OFFSET(AA9,0,-1),1+OFFSET(AA9,-1,0),1+OFFSET(AA9,-1,-1)))</f>
         <v>8</v>
       </c>
-      <c r="AA9" s="2"/>
       <c r="AB9" s="1"/>
       <c r="AC9" s="1"/>
       <c r="AD9" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>B</v>
       </c>
       <c r="AE9" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>B</v>
       </c>
       <c r="AF9" s="1"/>
@@ -1059,55 +1094,57 @@
       <c r="P10" s="3">
         <v>4</v>
       </c>
-      <c r="Q10" s="2" cm="1">
-        <f t="array" aca="1" ref="Q10" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(Q10,-1,-1),MIN(1+OFFSET(Q10,0,-1),1+OFFSET(Q10,-1,0),1+OFFSET(Q10,-1,-1)))</f>
+      <c r="Q10" s="2">
         <v>4</v>
       </c>
       <c r="R10" s="2" cm="1">
-        <f t="array" aca="1" ref="R10" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(R10,-1,-1),MIN(1+OFFSET(R10,0,-1),1+OFFSET(R10,-1,0),1+OFFSET(R10,-1,-1)))</f>
+        <f t="array" aca="1" ref="R10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,R$5+1,1),OFFSET(R10,-1,-1),MIN(1+OFFSET(R10,0,-1),1+OFFSET(R10,-1,0),1+OFFSET(R10,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="S10" s="2" cm="1">
-        <f t="array" aca="1" ref="S10" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(S10,-1,-1),MIN(1+OFFSET(S10,0,-1),1+OFFSET(S10,-1,0),1+OFFSET(S10,-1,-1)))</f>
+        <f t="array" aca="1" ref="S10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,S$5+1,1),OFFSET(S10,-1,-1),MIN(1+OFFSET(S10,0,-1),1+OFFSET(S10,-1,0),1+OFFSET(S10,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="T10" s="2" cm="1">
+        <f t="array" aca="1" ref="T10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,T$5+1,1),OFFSET(T10,-1,-1),MIN(1+OFFSET(T10,0,-1),1+OFFSET(T10,-1,0),1+OFFSET(T10,-1,-1)))</f>
         <v>3</v>
       </c>
-      <c r="T10" s="2" cm="1">
-        <f t="array" aca="1" ref="T10" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(T10,-1,-1),MIN(1+OFFSET(T10,0,-1),1+OFFSET(T10,-1,0),1+OFFSET(T10,-1,-1)))</f>
+      <c r="U10" s="2" cm="1">
+        <f t="array" aca="1" ref="U10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,U$5+1,1),OFFSET(U10,-1,-1),MIN(1+OFFSET(U10,0,-1),1+OFFSET(U10,-1,0),1+OFFSET(U10,-1,-1)))</f>
+        <v>2</v>
+      </c>
+      <c r="V10" s="2" cm="1">
+        <f t="array" aca="1" ref="V10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,V$5+1,1),OFFSET(V10,-1,-1),MIN(1+OFFSET(V10,0,-1),1+OFFSET(V10,-1,0),1+OFFSET(V10,-1,-1)))</f>
         <v>3</v>
       </c>
-      <c r="U10" s="2" cm="1">
-        <f t="array" aca="1" ref="U10" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(U10,-1,-1),MIN(1+OFFSET(U10,0,-1),1+OFFSET(U10,-1,0),1+OFFSET(U10,-1,-1)))</f>
-        <v>2</v>
-      </c>
-      <c r="V10" s="2" cm="1">
-        <f t="array" aca="1" ref="V10" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(V10,-1,-1),MIN(1+OFFSET(V10,0,-1),1+OFFSET(V10,-1,0),1+OFFSET(V10,-1,-1)))</f>
-        <v>3</v>
-      </c>
       <c r="W10" s="2" cm="1">
-        <f t="array" aca="1" ref="W10" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(W10,-1,-1),MIN(1+OFFSET(W10,0,-1),1+OFFSET(W10,-1,0),1+OFFSET(W10,-1,-1)))</f>
+        <f t="array" aca="1" ref="W10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,W$5+1,1),OFFSET(W10,-1,-1),MIN(1+OFFSET(W10,0,-1),1+OFFSET(W10,-1,0),1+OFFSET(W10,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="X10" s="2" cm="1">
-        <f t="array" aca="1" ref="X10" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(X10,-1,-1),MIN(1+OFFSET(X10,0,-1),1+OFFSET(X10,-1,0),1+OFFSET(X10,-1,-1)))</f>
+        <f t="array" aca="1" ref="X10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,X$5+1,1),OFFSET(X10,-1,-1),MIN(1+OFFSET(X10,0,-1),1+OFFSET(X10,-1,0),1+OFFSET(X10,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="Y10" s="2" cm="1">
-        <f t="array" aca="1" ref="Y10" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(Y10,-1,-1),MIN(1+OFFSET(Y10,0,-1),1+OFFSET(Y10,-1,0),1+OFFSET(Y10,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y10,-1,-1),MIN(1+OFFSET(Y10,0,-1),1+OFFSET(Y10,-1,0),1+OFFSET(Y10,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="Z10" s="2" cm="1">
-        <f t="array" aca="1" ref="Z10" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P10+1,1),OFFSET(Z10,-1,-1),MIN(1+OFFSET(Z10,0,-1),1+OFFSET(Z10,-1,0),1+OFFSET(Z10,-1,-1)))</f>
-        <v>7</v>
-      </c>
-      <c r="AA10" s="2"/>
+        <f t="array" aca="1" ref="Z10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z10,-1,-1),MIN(1+OFFSET(Z10,0,-1),1+OFFSET(Z10,-1,0),1+OFFSET(Z10,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="AA10" s="2" cm="1">
+        <f t="array" aca="1" ref="AA10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA10,-1,-1),MIN(1+OFFSET(AA10,0,-1),1+OFFSET(AA10,-1,0),1+OFFSET(AA10,-1,-1)))</f>
+        <v>8</v>
+      </c>
       <c r="AB10" s="1"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="AE10" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>C</v>
       </c>
       <c r="AF10" s="1"/>
@@ -1131,53 +1168,55 @@
       <c r="P11" s="3">
         <v>5</v>
       </c>
-      <c r="Q11" s="2" cm="1">
-        <f t="array" aca="1" ref="Q11" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(Q11,-1,-1),MIN(1+OFFSET(Q11,0,-1),1+OFFSET(Q11,-1,0),1+OFFSET(Q11,-1,-1)))</f>
+      <c r="Q11" s="2">
         <v>5</v>
       </c>
       <c r="R11" s="2" cm="1">
-        <f t="array" aca="1" ref="R11" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(R11,-1,-1),MIN(1+OFFSET(R11,0,-1),1+OFFSET(R11,-1,0),1+OFFSET(R11,-1,-1)))</f>
+        <f t="array" aca="1" ref="R11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,R$5+1,1),OFFSET(R11,-1,-1),MIN(1+OFFSET(R11,0,-1),1+OFFSET(R11,-1,0),1+OFFSET(R11,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="S11" s="2" cm="1">
-        <f t="array" aca="1" ref="S11" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(S11,-1,-1),MIN(1+OFFSET(S11,0,-1),1+OFFSET(S11,-1,0),1+OFFSET(S11,-1,-1)))</f>
+        <f t="array" aca="1" ref="S11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,S$5+1,1),OFFSET(S11,-1,-1),MIN(1+OFFSET(S11,0,-1),1+OFFSET(S11,-1,0),1+OFFSET(S11,-1,-1)))</f>
+        <v>5</v>
+      </c>
+      <c r="T11" s="2" cm="1">
+        <f t="array" aca="1" ref="T11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,T$5+1,1),OFFSET(T11,-1,-1),MIN(1+OFFSET(T11,0,-1),1+OFFSET(T11,-1,0),1+OFFSET(T11,-1,-1)))</f>
         <v>4</v>
       </c>
-      <c r="T11" s="2" cm="1">
-        <f t="array" aca="1" ref="T11" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(T11,-1,-1),MIN(1+OFFSET(T11,0,-1),1+OFFSET(T11,-1,0),1+OFFSET(T11,-1,-1)))</f>
+      <c r="U11" s="2" cm="1">
+        <f t="array" aca="1" ref="U11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,U$5+1,1),OFFSET(U11,-1,-1),MIN(1+OFFSET(U11,0,-1),1+OFFSET(U11,-1,0),1+OFFSET(U11,-1,-1)))</f>
+        <v>3</v>
+      </c>
+      <c r="V11" s="2" cm="1">
+        <f t="array" aca="1" ref="V11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,V$5+1,1),OFFSET(V11,-1,-1),MIN(1+OFFSET(V11,0,-1),1+OFFSET(V11,-1,0),1+OFFSET(V11,-1,-1)))</f>
+        <v>3</v>
+      </c>
+      <c r="W11" s="2" cm="1">
+        <f t="array" aca="1" ref="W11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,W$5+1,1),OFFSET(W11,-1,-1),MIN(1+OFFSET(W11,0,-1),1+OFFSET(W11,-1,0),1+OFFSET(W11,-1,-1)))</f>
         <v>4</v>
       </c>
-      <c r="U11" s="2" cm="1">
-        <f t="array" aca="1" ref="U11" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(U11,-1,-1),MIN(1+OFFSET(U11,0,-1),1+OFFSET(U11,-1,0),1+OFFSET(U11,-1,-1)))</f>
-        <v>3</v>
-      </c>
-      <c r="V11" s="2" cm="1">
-        <f t="array" aca="1" ref="V11" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(V11,-1,-1),MIN(1+OFFSET(V11,0,-1),1+OFFSET(V11,-1,0),1+OFFSET(V11,-1,-1)))</f>
-        <v>3</v>
-      </c>
-      <c r="W11" s="2" cm="1">
-        <f t="array" aca="1" ref="W11" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(W11,-1,-1),MIN(1+OFFSET(W11,0,-1),1+OFFSET(W11,-1,0),1+OFFSET(W11,-1,-1)))</f>
-        <v>4</v>
-      </c>
       <c r="X11" s="2" cm="1">
-        <f t="array" aca="1" ref="X11" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(X11,-1,-1),MIN(1+OFFSET(X11,0,-1),1+OFFSET(X11,-1,0),1+OFFSET(X11,-1,-1)))</f>
+        <f t="array" aca="1" ref="X11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,X$5+1,1),OFFSET(X11,-1,-1),MIN(1+OFFSET(X11,0,-1),1+OFFSET(X11,-1,0),1+OFFSET(X11,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="Y11" s="2" cm="1">
-        <f t="array" aca="1" ref="Y11" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(Y11,-1,-1),MIN(1+OFFSET(Y11,0,-1),1+OFFSET(Y11,-1,0),1+OFFSET(Y11,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="Y11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y11,-1,-1),MIN(1+OFFSET(Y11,0,-1),1+OFFSET(Y11,-1,0),1+OFFSET(Y11,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="Z11" s="2" cm="1">
-        <f t="array" aca="1" ref="Z11" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P11+1,1),OFFSET(Z11,-1,-1),MIN(1+OFFSET(Z11,0,-1),1+OFFSET(Z11,-1,0),1+OFFSET(Z11,-1,-1)))</f>
-        <v>7</v>
-      </c>
-      <c r="AA11" s="2"/>
+        <f t="array" aca="1" ref="Z11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z11,-1,-1),MIN(1+OFFSET(Z11,0,-1),1+OFFSET(Z11,-1,0),1+OFFSET(Z11,-1,-1)))</f>
+        <v>6</v>
+      </c>
+      <c r="AA11" s="2" cm="1">
+        <f t="array" aca="1" ref="AA11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA11,-1,-1),MIN(1+OFFSET(AA11,0,-1),1+OFFSET(AA11,-1,0),1+OFFSET(AA11,-1,-1)))</f>
+        <v>7</v>
+      </c>
       <c r="AD11" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>E</v>
       </c>
       <c r="AE11" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>D</v>
       </c>
     </row>
@@ -1200,53 +1239,55 @@
       <c r="P12" s="3">
         <v>6</v>
       </c>
-      <c r="Q12" s="2" cm="1">
-        <f t="array" aca="1" ref="Q12" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(Q12,-1,-1),MIN(1+OFFSET(Q12,0,-1),1+OFFSET(Q12,-1,0),1+OFFSET(Q12,-1,-1)))</f>
+      <c r="Q12" s="2">
         <v>6</v>
       </c>
       <c r="R12" s="2" cm="1">
-        <f t="array" aca="1" ref="R12" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(R12,-1,-1),MIN(1+OFFSET(R12,0,-1),1+OFFSET(R12,-1,0),1+OFFSET(R12,-1,-1)))</f>
+        <f t="array" aca="1" ref="R12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,R$5+1,1),OFFSET(R12,-1,-1),MIN(1+OFFSET(R12,0,-1),1+OFFSET(R12,-1,0),1+OFFSET(R12,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="S12" s="2" cm="1">
-        <f t="array" aca="1" ref="S12" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(S12,-1,-1),MIN(1+OFFSET(S12,0,-1),1+OFFSET(S12,-1,0),1+OFFSET(S12,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="S12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,S$5+1,1),OFFSET(S12,-1,-1),MIN(1+OFFSET(S12,0,-1),1+OFFSET(S12,-1,0),1+OFFSET(S12,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="T12" s="2" cm="1">
-        <f t="array" aca="1" ref="T12" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(T12,-1,-1),MIN(1+OFFSET(T12,0,-1),1+OFFSET(T12,-1,0),1+OFFSET(T12,-1,-1)))</f>
+        <f t="array" aca="1" ref="T12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,T$5+1,1),OFFSET(T12,-1,-1),MIN(1+OFFSET(T12,0,-1),1+OFFSET(T12,-1,0),1+OFFSET(T12,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="U12" s="2" cm="1">
-        <f t="array" aca="1" ref="U12" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(U12,-1,-1),MIN(1+OFFSET(U12,0,-1),1+OFFSET(U12,-1,0),1+OFFSET(U12,-1,-1)))</f>
+        <f t="array" aca="1" ref="U12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,U$5+1,1),OFFSET(U12,-1,-1),MIN(1+OFFSET(U12,0,-1),1+OFFSET(U12,-1,0),1+OFFSET(U12,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="V12" s="2" cm="1">
-        <f t="array" aca="1" ref="V12" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(V12,-1,-1),MIN(1+OFFSET(V12,0,-1),1+OFFSET(V12,-1,0),1+OFFSET(V12,-1,-1)))</f>
+        <f t="array" aca="1" ref="V12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,V$5+1,1),OFFSET(V12,-1,-1),MIN(1+OFFSET(V12,0,-1),1+OFFSET(V12,-1,0),1+OFFSET(V12,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="W12" s="2" cm="1">
-        <f t="array" aca="1" ref="W12" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(W12,-1,-1),MIN(1+OFFSET(W12,0,-1),1+OFFSET(W12,-1,0),1+OFFSET(W12,-1,-1)))</f>
+        <f t="array" aca="1" ref="W12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,W$5+1,1),OFFSET(W12,-1,-1),MIN(1+OFFSET(W12,0,-1),1+OFFSET(W12,-1,0),1+OFFSET(W12,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="X12" s="2" cm="1">
-        <f t="array" aca="1" ref="X12" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(X12,-1,-1),MIN(1+OFFSET(X12,0,-1),1+OFFSET(X12,-1,0),1+OFFSET(X12,-1,-1)))</f>
-        <v>4</v>
+        <f t="array" aca="1" ref="X12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,X$5+1,1),OFFSET(X12,-1,-1),MIN(1+OFFSET(X12,0,-1),1+OFFSET(X12,-1,0),1+OFFSET(X12,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="Y12" s="2" cm="1">
-        <f t="array" aca="1" ref="Y12" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(Y12,-1,-1),MIN(1+OFFSET(Y12,0,-1),1+OFFSET(Y12,-1,0),1+OFFSET(Y12,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="Y12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y12,-1,-1),MIN(1+OFFSET(Y12,0,-1),1+OFFSET(Y12,-1,0),1+OFFSET(Y12,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="Z12" s="2" cm="1">
-        <f t="array" aca="1" ref="Z12" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P12+1,1),OFFSET(Z12,-1,-1),MIN(1+OFFSET(Z12,0,-1),1+OFFSET(Z12,-1,0),1+OFFSET(Z12,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="AA12" s="2"/>
+        <f t="array" aca="1" ref="Z12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z12,-1,-1),MIN(1+OFFSET(Z12,0,-1),1+OFFSET(Z12,-1,0),1+OFFSET(Z12,-1,-1)))</f>
+        <v>5</v>
+      </c>
+      <c r="AA12" s="2" cm="1">
+        <f t="array" aca="1" ref="AA12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA12,-1,-1),MIN(1+OFFSET(AA12,0,-1),1+OFFSET(AA12,-1,0),1+OFFSET(AA12,-1,-1)))</f>
+        <v>6</v>
+      </c>
       <c r="AD12" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>F</v>
       </c>
       <c r="AE12" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
     </row>
@@ -1269,53 +1310,55 @@
       <c r="P13" s="3">
         <v>7</v>
       </c>
-      <c r="Q13" s="2" cm="1">
-        <f t="array" aca="1" ref="Q13" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(Q13,-1,-1),MIN(1+OFFSET(Q13,0,-1),1+OFFSET(Q13,-1,0),1+OFFSET(Q13,-1,-1)))</f>
+      <c r="Q13" s="2">
         <v>7</v>
       </c>
       <c r="R13" s="2" cm="1">
-        <f t="array" aca="1" ref="R13" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(R13,-1,-1),MIN(1+OFFSET(R13,0,-1),1+OFFSET(R13,-1,0),1+OFFSET(R13,-1,-1)))</f>
+        <f t="array" aca="1" ref="R13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,R$5+1,1),OFFSET(R13,-1,-1),MIN(1+OFFSET(R13,0,-1),1+OFFSET(R13,-1,0),1+OFFSET(R13,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="S13" s="2" cm="1">
-        <f t="array" aca="1" ref="S13" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(S13,-1,-1),MIN(1+OFFSET(S13,0,-1),1+OFFSET(S13,-1,0),1+OFFSET(S13,-1,-1)))</f>
+        <f t="array" aca="1" ref="S13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,S$5+1,1),OFFSET(S13,-1,-1),MIN(1+OFFSET(S13,0,-1),1+OFFSET(S13,-1,0),1+OFFSET(S13,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="T13" s="2" cm="1">
-        <f t="array" aca="1" ref="T13" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(T13,-1,-1),MIN(1+OFFSET(T13,0,-1),1+OFFSET(T13,-1,0),1+OFFSET(T13,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="T13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,T$5+1,1),OFFSET(T13,-1,-1),MIN(1+OFFSET(T13,0,-1),1+OFFSET(T13,-1,0),1+OFFSET(T13,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="U13" s="2" cm="1">
-        <f t="array" aca="1" ref="U13" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(U13,-1,-1),MIN(1+OFFSET(U13,0,-1),1+OFFSET(U13,-1,0),1+OFFSET(U13,-1,-1)))</f>
+        <f t="array" aca="1" ref="U13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,U$5+1,1),OFFSET(U13,-1,-1),MIN(1+OFFSET(U13,0,-1),1+OFFSET(U13,-1,0),1+OFFSET(U13,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="V13" s="2" cm="1">
-        <f t="array" aca="1" ref="V13" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(V13,-1,-1),MIN(1+OFFSET(V13,0,-1),1+OFFSET(V13,-1,0),1+OFFSET(V13,-1,-1)))</f>
+        <f t="array" aca="1" ref="V13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,V$5+1,1),OFFSET(V13,-1,-1),MIN(1+OFFSET(V13,0,-1),1+OFFSET(V13,-1,0),1+OFFSET(V13,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="W13" s="2" cm="1">
-        <f t="array" aca="1" ref="W13" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(W13,-1,-1),MIN(1+OFFSET(W13,0,-1),1+OFFSET(W13,-1,0),1+OFFSET(W13,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="W13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,W$5+1,1),OFFSET(W13,-1,-1),MIN(1+OFFSET(W13,0,-1),1+OFFSET(W13,-1,0),1+OFFSET(W13,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="X13" s="2" cm="1">
-        <f t="array" aca="1" ref="X13" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(X13,-1,-1),MIN(1+OFFSET(X13,0,-1),1+OFFSET(X13,-1,0),1+OFFSET(X13,-1,-1)))</f>
+        <f t="array" aca="1" ref="X13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,X$5+1,1),OFFSET(X13,-1,-1),MIN(1+OFFSET(X13,0,-1),1+OFFSET(X13,-1,0),1+OFFSET(X13,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="Y13" s="2" cm="1">
-        <f t="array" aca="1" ref="Y13" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(Y13,-1,-1),MIN(1+OFFSET(Y13,0,-1),1+OFFSET(Y13,-1,0),1+OFFSET(Y13,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="Y13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y13,-1,-1),MIN(1+OFFSET(Y13,0,-1),1+OFFSET(Y13,-1,0),1+OFFSET(Y13,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="Z13" s="2" cm="1">
-        <f t="array" aca="1" ref="Z13" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P13+1,1),OFFSET(Z13,-1,-1),MIN(1+OFFSET(Z13,0,-1),1+OFFSET(Z13,-1,0),1+OFFSET(Z13,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="AA13" s="2"/>
+        <f t="array" aca="1" ref="Z13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z13,-1,-1),MIN(1+OFFSET(Z13,0,-1),1+OFFSET(Z13,-1,0),1+OFFSET(Z13,-1,-1)))</f>
+        <v>6</v>
+      </c>
+      <c r="AA13" s="2" cm="1">
+        <f t="array" aca="1" ref="AA13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA13,-1,-1),MIN(1+OFFSET(AA13,0,-1),1+OFFSET(AA13,-1,0),1+OFFSET(AA13,-1,-1)))</f>
+        <v>5</v>
+      </c>
       <c r="AD13" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
       <c r="AE13" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>B</v>
       </c>
     </row>
@@ -1338,53 +1381,55 @@
       <c r="P14" s="3">
         <v>8</v>
       </c>
-      <c r="Q14" s="2" cm="1">
-        <f t="array" aca="1" ref="Q14" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(Q14,-1,-1),MIN(1+OFFSET(Q14,0,-1),1+OFFSET(Q14,-1,0),1+OFFSET(Q14,-1,-1)))</f>
+      <c r="Q14" s="2">
         <v>8</v>
       </c>
       <c r="R14" s="2" cm="1">
-        <f t="array" aca="1" ref="R14" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(R14,-1,-1),MIN(1+OFFSET(R14,0,-1),1+OFFSET(R14,-1,0),1+OFFSET(R14,-1,-1)))</f>
+        <f t="array" aca="1" ref="R14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,R$5+1,1),OFFSET(R14,-1,-1),MIN(1+OFFSET(R14,0,-1),1+OFFSET(R14,-1,0),1+OFFSET(R14,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="S14" s="2" cm="1">
-        <f t="array" aca="1" ref="S14" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(S14,-1,-1),MIN(1+OFFSET(S14,0,-1),1+OFFSET(S14,-1,0),1+OFFSET(S14,-1,-1)))</f>
+        <f t="array" aca="1" ref="S14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,S$5+1,1),OFFSET(S14,-1,-1),MIN(1+OFFSET(S14,0,-1),1+OFFSET(S14,-1,0),1+OFFSET(S14,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="T14" s="2" cm="1">
-        <f t="array" aca="1" ref="T14" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(T14,-1,-1),MIN(1+OFFSET(T14,0,-1),1+OFFSET(T14,-1,0),1+OFFSET(T14,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="T14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,T$5+1,1),OFFSET(T14,-1,-1),MIN(1+OFFSET(T14,0,-1),1+OFFSET(T14,-1,0),1+OFFSET(T14,-1,-1)))</f>
+        <v>7</v>
       </c>
       <c r="U14" s="2" cm="1">
-        <f t="array" aca="1" ref="U14" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(U14,-1,-1),MIN(1+OFFSET(U14,0,-1),1+OFFSET(U14,-1,0),1+OFFSET(U14,-1,-1)))</f>
+        <f t="array" aca="1" ref="U14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,U$5+1,1),OFFSET(U14,-1,-1),MIN(1+OFFSET(U14,0,-1),1+OFFSET(U14,-1,0),1+OFFSET(U14,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="V14" s="2" cm="1">
-        <f t="array" aca="1" ref="V14" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(V14,-1,-1),MIN(1+OFFSET(V14,0,-1),1+OFFSET(V14,-1,0),1+OFFSET(V14,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="V14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,V$5+1,1),OFFSET(V14,-1,-1),MIN(1+OFFSET(V14,0,-1),1+OFFSET(V14,-1,0),1+OFFSET(V14,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="W14" s="2" cm="1">
-        <f t="array" aca="1" ref="W14" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(W14,-1,-1),MIN(1+OFFSET(W14,0,-1),1+OFFSET(W14,-1,0),1+OFFSET(W14,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="W14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,W$5+1,1),OFFSET(W14,-1,-1),MIN(1+OFFSET(W14,0,-1),1+OFFSET(W14,-1,0),1+OFFSET(W14,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="X14" s="2" cm="1">
-        <f t="array" aca="1" ref="X14" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(X14,-1,-1),MIN(1+OFFSET(X14,0,-1),1+OFFSET(X14,-1,0),1+OFFSET(X14,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="X14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,X$5+1,1),OFFSET(X14,-1,-1),MIN(1+OFFSET(X14,0,-1),1+OFFSET(X14,-1,0),1+OFFSET(X14,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="Y14" s="2" cm="1">
-        <f t="array" aca="1" ref="Y14" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(Y14,-1,-1),MIN(1+OFFSET(Y14,0,-1),1+OFFSET(Y14,-1,0),1+OFFSET(Y14,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y14,-1,-1),MIN(1+OFFSET(Y14,0,-1),1+OFFSET(Y14,-1,0),1+OFFSET(Y14,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="Z14" s="2" cm="1">
-        <f t="array" aca="1" ref="Z14" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P14+1,1),OFFSET(Z14,-1,-1),MIN(1+OFFSET(Z14,0,-1),1+OFFSET(Z14,-1,0),1+OFFSET(Z14,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="AA14" s="2"/>
+        <f t="array" aca="1" ref="Z14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z14,-1,-1),MIN(1+OFFSET(Z14,0,-1),1+OFFSET(Z14,-1,0),1+OFFSET(Z14,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="AA14" s="2" cm="1">
+        <f t="array" aca="1" ref="AA14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA14,-1,-1),MIN(1+OFFSET(AA14,0,-1),1+OFFSET(AA14,-1,0),1+OFFSET(AA14,-1,-1)))</f>
+        <v>6</v>
+      </c>
       <c r="AD14" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>T</v>
       </c>
       <c r="AE14" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>E</v>
       </c>
     </row>
@@ -1412,102 +1457,78 @@
         <v>9</v>
       </c>
       <c r="R15" s="2" cm="1">
-        <f t="array" aca="1" ref="R15" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(R15,-1,-1),MIN(1+OFFSET(R15,0,-1),1+OFFSET(R15,-1,0),1+OFFSET(R15,-1,-1)))</f>
+        <f t="array" aca="1" ref="R15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,R$5+1,1),OFFSET(R15,-1,-1),MIN(1+OFFSET(R15,0,-1),1+OFFSET(R15,-1,0),1+OFFSET(R15,-1,-1)))</f>
         <v>9</v>
       </c>
       <c r="S15" s="2" cm="1">
-        <f t="array" aca="1" ref="S15" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(S15,-1,-1),MIN(1+OFFSET(S15,0,-1),1+OFFSET(S15,-1,0),1+OFFSET(S15,-1,-1)))</f>
+        <f t="array" aca="1" ref="S15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,S$5+1,1),OFFSET(S15,-1,-1),MIN(1+OFFSET(S15,0,-1),1+OFFSET(S15,-1,0),1+OFFSET(S15,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="T15" s="2" cm="1">
-        <f t="array" aca="1" ref="T15" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(T15,-1,-1),MIN(1+OFFSET(T15,0,-1),1+OFFSET(T15,-1,0),1+OFFSET(T15,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="T15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,T$5+1,1),OFFSET(T15,-1,-1),MIN(1+OFFSET(T15,0,-1),1+OFFSET(T15,-1,0),1+OFFSET(T15,-1,-1)))</f>
+        <v>8</v>
       </c>
       <c r="U15" s="2" cm="1">
-        <f t="array" aca="1" ref="U15" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(U15,-1,-1),MIN(1+OFFSET(U15,0,-1),1+OFFSET(U15,-1,0),1+OFFSET(U15,-1,-1)))</f>
+        <f t="array" aca="1" ref="U15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,U$5+1,1),OFFSET(U15,-1,-1),MIN(1+OFFSET(U15,0,-1),1+OFFSET(U15,-1,0),1+OFFSET(U15,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="V15" s="2" cm="1">
-        <f t="array" aca="1" ref="V15" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(V15,-1,-1),MIN(1+OFFSET(V15,0,-1),1+OFFSET(V15,-1,0),1+OFFSET(V15,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="V15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,V$5+1,1),OFFSET(V15,-1,-1),MIN(1+OFFSET(V15,0,-1),1+OFFSET(V15,-1,0),1+OFFSET(V15,-1,-1)))</f>
+        <v>7</v>
       </c>
       <c r="W15" s="2" cm="1">
-        <f t="array" aca="1" ref="W15" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(W15,-1,-1),MIN(1+OFFSET(W15,0,-1),1+OFFSET(W15,-1,0),1+OFFSET(W15,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="W15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,W$5+1,1),OFFSET(W15,-1,-1),MIN(1+OFFSET(W15,0,-1),1+OFFSET(W15,-1,0),1+OFFSET(W15,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="X15" s="2" cm="1">
-        <f t="array" aca="1" ref="X15" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(X15,-1,-1),MIN(1+OFFSET(X15,0,-1),1+OFFSET(X15,-1,0),1+OFFSET(X15,-1,-1)))</f>
+        <f t="array" aca="1" ref="X15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,X$5+1,1),OFFSET(X15,-1,-1),MIN(1+OFFSET(X15,0,-1),1+OFFSET(X15,-1,0),1+OFFSET(X15,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="Y15" s="2" cm="1">
-        <f t="array" aca="1" ref="Y15" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(Y15,-1,-1),MIN(1+OFFSET(Y15,0,-1),1+OFFSET(Y15,-1,0),1+OFFSET(Y15,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="Y15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y15,-1,-1),MIN(1+OFFSET(Y15,0,-1),1+OFFSET(Y15,-1,0),1+OFFSET(Y15,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="Z15" s="2" cm="1">
-        <f t="array" aca="1" ref="Z15" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(Z15,-1,-1),MIN(1+OFFSET(Z15,0,-1),1+OFFSET(Z15,-1,0),1+OFFSET(Z15,-1,-1)))</f>
-        <v>7</v>
-      </c>
-      <c r="AA15" s="2"/>
+        <f t="array" aca="1" ref="Z15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z15,-1,-1),MIN(1+OFFSET(Z15,0,-1),1+OFFSET(Z15,-1,0),1+OFFSET(Z15,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="AA15" s="2" cm="1">
+        <f t="array" aca="1" ref="AA15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA15,-1,-1),MIN(1+OFFSET(AA15,0,-1),1+OFFSET(AA15,-1,0),1+OFFSET(AA15,-1,-1)))</f>
+        <v>7</v>
+      </c>
       <c r="AD15" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>Z</v>
       </c>
       <c r="AE15" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>F</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O16" s="10" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="P16" s="3">
         <v>10</v>
       </c>
-      <c r="Q16" s="2" cm="1">
-        <f t="array" aca="1" ref="Q16" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(Q16,-1,-1),MIN(1+OFFSET(Q16,0,-1),1+OFFSET(Q16,-1,0),1+OFFSET(Q16,-1,-1)))</f>
-        <v>10</v>
-      </c>
-      <c r="R16" s="2" cm="1">
-        <f t="array" aca="1" ref="R16" ca="1">IF(INDEX(X,R$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(R16,-1,-1),MIN(1+OFFSET(R16,0,-1),1+OFFSET(R16,-1,0),1+OFFSET(R16,-1,-1)))</f>
-        <v>10</v>
-      </c>
-      <c r="S16" s="2" cm="1">
-        <f t="array" aca="1" ref="S16" ca="1">IF(INDEX(X,S$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(S16,-1,-1),MIN(1+OFFSET(S16,0,-1),1+OFFSET(S16,-1,0),1+OFFSET(S16,-1,-1)))</f>
-        <v>9</v>
-      </c>
-      <c r="T16" s="2" cm="1">
-        <f t="array" aca="1" ref="T16" ca="1">IF(INDEX(X,T$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(T16,-1,-1),MIN(1+OFFSET(T16,0,-1),1+OFFSET(T16,-1,0),1+OFFSET(T16,-1,-1)))</f>
-        <v>8</v>
-      </c>
-      <c r="U16" s="2" cm="1">
-        <f t="array" aca="1" ref="U16" ca="1">IF(INDEX(X,U$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(U16,-1,-1),MIN(1+OFFSET(U16,0,-1),1+OFFSET(U16,-1,0),1+OFFSET(U16,-1,-1)))</f>
-        <v>8</v>
-      </c>
-      <c r="V16" s="2" cm="1">
-        <f t="array" aca="1" ref="V16" ca="1">IF(INDEX(X,V$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(V16,-1,-1),MIN(1+OFFSET(V16,0,-1),1+OFFSET(V16,-1,0),1+OFFSET(V16,-1,-1)))</f>
-        <v>7</v>
-      </c>
-      <c r="W16" s="2" cm="1">
-        <f t="array" aca="1" ref="W16" ca="1">IF(INDEX(X,W$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(W16,-1,-1),MIN(1+OFFSET(W16,0,-1),1+OFFSET(W16,-1,0),1+OFFSET(W16,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="X16" s="2" cm="1">
-        <f t="array" aca="1" ref="X16" ca="1">IF(INDEX(X,X$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(X16,-1,-1),MIN(1+OFFSET(X16,0,-1),1+OFFSET(X16,-1,0),1+OFFSET(X16,-1,-1)))</f>
-        <v>5</v>
-      </c>
-      <c r="Y16" s="2" cm="1">
-        <f t="array" aca="1" ref="Y16" ca="1">IF(INDEX(X,Y$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(Y16,-1,-1),MIN(1+OFFSET(Y16,0,-1),1+OFFSET(Y16,-1,0),1+OFFSET(Y16,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="Z16" s="2" cm="1">
-        <f t="array" aca="1" ref="Z16" ca="1">IF(INDEX(X,Z$5+1,1)=INDEX(Y,$P16+1,1),OFFSET(Z16,-1,-1),MIN(1+OFFSET(Z16,0,-1),1+OFFSET(Z16,-1,0),1+OFFSET(Z16,-1,-1)))</f>
-        <v>7</v>
-      </c>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="2"/>
+      <c r="S16" s="2"/>
+      <c r="T16" s="2"/>
+      <c r="U16" s="2"/>
+      <c r="V16" s="2"/>
+      <c r="W16" s="2"/>
+      <c r="X16" s="2"/>
+      <c r="Y16" s="2"/>
+      <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
-      <c r="AD16" s="8"/>
+      <c r="AD16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
       <c r="AE16" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>A</v>
       </c>
     </row>
@@ -1528,15 +1549,15 @@
     <row r="18" spans="16:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="AC18" s="6"/>
       <c r="AD18" s="8">
-        <f>COUNTA(AD7:AD16)</f>
+        <f>COUNTIFS(AD$7:AD$16,"?")</f>
         <v>9</v>
       </c>
       <c r="AE18" s="8">
-        <f>COUNTA(AE7:AE16)</f>
+        <f>COUNTIFS(AE$7:AE$16,"?")</f>
         <v>10</v>
       </c>
       <c r="AF18" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1544,8 +1565,8 @@
     <mergeCell ref="AD4:AE4"/>
   </mergeCells>
   <conditionalFormatting sqref="Q6:AA16">
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>"OFFSET($C$9;$T$8;$S$8)"</formula>
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND($P6=$AD$18,Q$5=$AE$18)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Try test case 2 to trace operators but fails -> continue study
</commit_message>
<xml_diff>
--- a/DynamicPro/editDistance/editDistance.xlsx
+++ b/DynamicPro/editDistance/editDistance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoikhang/Documents/SWCPT/DynamicPro/editDistance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32D0A90-7293-2146-B964-64A1064C908E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86350BEF-CF11-C343-B49C-E43BBCD40FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,10 @@
     <definedName name="Fij">Sheet1!$Q$6:$AA$16</definedName>
     <definedName name="i">Sheet1!$P$6:$P$16</definedName>
     <definedName name="j">Sheet1!$Q$5:$AA$5</definedName>
-    <definedName name="vi">Sheet1!$AE$6:$AE$16</definedName>
+    <definedName name="vi">Sheet1!$AF$6:$AF$16</definedName>
     <definedName name="wi">Sheet1!$P$6:$P$16</definedName>
-    <definedName name="X">Sheet1!$AD$6:$AD$15</definedName>
-    <definedName name="Y">Sheet1!$AE$6:$AE$16</definedName>
+    <definedName name="X">Sheet1!$AE$7:$AE$16</definedName>
+    <definedName name="Y">Sheet1!$AF$7:$AF$16</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>B2</t>
   </si>
@@ -138,13 +138,76 @@
     <t>PBBCEFATZ</t>
   </si>
   <si>
-    <t>QABCDABEFA</t>
-  </si>
-  <si>
-    <t>X &lt;--</t>
-  </si>
-  <si>
-    <t>--&gt;Y</t>
+    <t>FOOD</t>
+  </si>
+  <si>
+    <t>MONEY</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Z</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>PBBCEFATZA</t>
+  </si>
+  <si>
+    <t>PBBCEFATZAF</t>
+  </si>
+  <si>
+    <t>PBBCEFATAF</t>
+  </si>
+  <si>
+    <t>i=8;j=8</t>
+  </si>
+  <si>
+    <t>i=8;j=7</t>
+  </si>
+  <si>
+    <t>inser(A)</t>
+  </si>
+  <si>
+    <t>inser(F)</t>
+  </si>
+  <si>
+    <t>del(Z)</t>
+  </si>
+  <si>
+    <t>i=7;j=7</t>
+  </si>
+  <si>
+    <t>insert(E.)</t>
+  </si>
+  <si>
+    <t>PBBCEFATEAF</t>
+  </si>
+  <si>
+    <t>i=7;j=6</t>
+  </si>
+  <si>
+    <t>Y &lt;--</t>
+  </si>
+  <si>
+    <t>--&gt;X</t>
   </si>
 </sst>
 </file>
@@ -162,6 +225,7 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -273,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -291,7 +355,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -314,20 +377,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -335,26 +405,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -582,10 +632,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AH18"/>
+  <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="125" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -595,129 +645,130 @@
     <col min="3" max="3" width="3.5" customWidth="1"/>
     <col min="4" max="13" width="3.6640625" customWidth="1"/>
     <col min="14" max="14" width="4.1640625" customWidth="1"/>
-    <col min="15" max="27" width="5" customWidth="1"/>
-    <col min="28" max="28" width="6" customWidth="1"/>
-    <col min="29" max="29" width="6.33203125" customWidth="1"/>
-    <col min="30" max="30" width="11.33203125" style="19" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="26" width="5" customWidth="1"/>
+    <col min="27" max="28" width="7.5" customWidth="1"/>
+    <col min="29" max="29" width="6" customWidth="1"/>
+    <col min="30" max="30" width="6.33203125" customWidth="1"/>
+    <col min="31" max="32" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="13" t="s">
+    <row r="1" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="12"/>
+      <c r="P1" s="11"/>
       <c r="R1" s="1"/>
     </row>
-    <row r="2" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="13" t="s">
+    <row r="2" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="12"/>
+      <c r="P2" s="11"/>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:34" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+    <row r="3" spans="1:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
-      <c r="O4" s="13"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="12"/>
       <c r="P4" s="6" t="s">
         <v>4</v>
       </c>
       <c r="AA4" s="6"/>
-      <c r="AB4" s="1"/>
+      <c r="AB4" s="6"/>
       <c r="AC4" s="1"/>
-      <c r="AD4" s="20" t="s">
+      <c r="AD4" s="1"/>
+      <c r="AE4" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="AE4" s="21"/>
-      <c r="AF4" s="6"/>
+      <c r="AF4" s="21"/>
       <c r="AG4" s="6"/>
       <c r="AH4" s="6"/>
-    </row>
-    <row r="5" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="13" t="s">
+      <c r="AI4" s="6"/>
+    </row>
+    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="18"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="17"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3">
         <v>0</v>
@@ -752,40 +803,41 @@
       <c r="AA5" s="3">
         <v>10</v>
       </c>
-      <c r="AB5" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="7" t="s">
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="AE5" s="7" t="s">
+      <c r="AF5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="AF5" s="6"/>
       <c r="AG5" s="6"/>
       <c r="AH5" s="6"/>
-    </row>
-    <row r="6" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
+      <c r="AI5" s="6"/>
+    </row>
+    <row r="6" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="13"/>
       <c r="P6" s="3">
         <v>0</v>
       </c>
@@ -822,39 +874,36 @@
       <c r="AA6" s="2">
         <v>10</v>
       </c>
-      <c r="AD6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AE6" s="22" t="s">
+      <c r="AB6" s="24"/>
+      <c r="AE6" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AF6" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG6" s="22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
+      <c r="AF6" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG6" s="7"/>
+      <c r="AH6" s="19"/>
+    </row>
+    <row r="7" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="14"/>
-      <c r="M7" s="14"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="14"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="13"/>
+      <c r="N7" s="13"/>
+      <c r="O7" s="13"/>
       <c r="P7" s="3">
         <v>1</v>
       </c>
@@ -862,79 +911,85 @@
         <v>1</v>
       </c>
       <c r="R7" s="2" cm="1">
-        <f t="array" aca="1" ref="R7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,R$5+1,1),OFFSET(R7,-1,-1),MIN(1+OFFSET(R7,0,-1),1+OFFSET(R7,-1,0),1+OFFSET(R7,-1,-1)))</f>
+        <f t="array" aca="1" ref="R7" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P7,0),OFFSET(R7,-1,-1),MIN(1+OFFSET(R7,-1,0),1+OFFSET(R7,0,-1),1+OFFSET(R7,-1,-1)))</f>
         <v>1</v>
       </c>
       <c r="S7" s="2" cm="1">
-        <f t="array" aca="1" ref="S7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,S$5+1,1),OFFSET(S7,-1,-1),MIN(1+OFFSET(S7,0,-1),1+OFFSET(S7,-1,0),1+OFFSET(S7,-1,-1)))</f>
+        <f t="array" aca="1" ref="S7" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P7,0),OFFSET(S7,-1,-1),MIN(1+OFFSET(S7,-1,0),1+OFFSET(S7,0,-1),1+OFFSET(S7,-1,-1)))</f>
         <v>2</v>
       </c>
       <c r="T7" s="2" cm="1">
-        <f t="array" aca="1" ref="T7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,T$5+1,1),OFFSET(T7,-1,-1),MIN(1+OFFSET(T7,0,-1),1+OFFSET(T7,-1,0),1+OFFSET(T7,-1,-1)))</f>
+        <f t="array" aca="1" ref="T7" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P7,0),OFFSET(T7,-1,-1),MIN(1+OFFSET(T7,-1,0),1+OFFSET(T7,0,-1),1+OFFSET(T7,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="U7" s="2" cm="1">
-        <f t="array" aca="1" ref="U7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,U$5+1,1),OFFSET(U7,-1,-1),MIN(1+OFFSET(U7,0,-1),1+OFFSET(U7,-1,0),1+OFFSET(U7,-1,-1)))</f>
+        <f t="array" aca="1" ref="U7" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P7,0),OFFSET(U7,-1,-1),MIN(1+OFFSET(U7,-1,0),1+OFFSET(U7,0,-1),1+OFFSET(U7,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="V7" s="2" cm="1">
-        <f t="array" aca="1" ref="V7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,V$5+1,1),OFFSET(V7,-1,-1),MIN(1+OFFSET(V7,0,-1),1+OFFSET(V7,-1,0),1+OFFSET(V7,-1,-1)))</f>
+        <f t="array" aca="1" ref="V7" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P7,0),OFFSET(V7,-1,-1),MIN(1+OFFSET(V7,-1,0),1+OFFSET(V7,0,-1),1+OFFSET(V7,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="W7" s="2" cm="1">
-        <f t="array" aca="1" ref="W7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,W$5+1,1),OFFSET(W7,-1,-1),MIN(1+OFFSET(W7,0,-1),1+OFFSET(W7,-1,0),1+OFFSET(W7,-1,-1)))</f>
+        <f t="array" aca="1" ref="W7" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P7,0),OFFSET(W7,-1,-1),MIN(1+OFFSET(W7,-1,0),1+OFFSET(W7,0,-1),1+OFFSET(W7,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="X7" s="2" cm="1">
-        <f t="array" aca="1" ref="X7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,X$5+1,1),OFFSET(X7,-1,-1),MIN(1+OFFSET(X7,0,-1),1+OFFSET(X7,-1,0),1+OFFSET(X7,-1,-1)))</f>
+        <f t="array" aca="1" ref="X7" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P7,0),OFFSET(X7,-1,-1),MIN(1+OFFSET(X7,-1,0),1+OFFSET(X7,0,-1),1+OFFSET(X7,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="Y7" s="2" cm="1">
-        <f t="array" aca="1" ref="Y7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y7,-1,-1),MIN(1+OFFSET(Y7,0,-1),1+OFFSET(Y7,-1,0),1+OFFSET(Y7,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y7" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P7,0),OFFSET(Y7,-1,-1),MIN(1+OFFSET(Y7,-1,0),1+OFFSET(Y7,0,-1),1+OFFSET(Y7,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="Z7" s="2" cm="1">
-        <f t="array" aca="1" ref="Z7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z7,-1,-1),MIN(1+OFFSET(Z7,0,-1),1+OFFSET(Z7,-1,0),1+OFFSET(Z7,-1,-1)))</f>
+        <f t="array" aca="1" ref="Z7" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P7,0),OFFSET(Z7,-1,-1),MIN(1+OFFSET(Z7,-1,0),1+OFFSET(Z7,0,-1),1+OFFSET(Z7,-1,-1)))</f>
         <v>9</v>
       </c>
       <c r="AA7" s="2" cm="1">
-        <f t="array" aca="1" ref="AA7" ca="1">IF(INDEX(X,$P7+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA7,-1,-1),MIN(1+OFFSET(AA7,0,-1),1+OFFSET(AA7,-1,0),1+OFFSET(AA7,-1,-1)))</f>
+        <f t="array" aca="1" ref="AA7" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P7,0),OFFSET(AA7,-1,-1),MIN(1+OFFSET(AA7,-1,0),1+OFFSET(AA7,0,-1),1+OFFSET(AA7,-1,-1)))</f>
         <v>10</v>
       </c>
-      <c r="AB7" s="1"/>
+      <c r="AB7" s="24"/>
       <c r="AC7" s="1"/>
-      <c r="AD7" s="7" t="str">
-        <f>MID(AD$6,$P7,1)</f>
-        <v>P</v>
-      </c>
+      <c r="AD7" s="1"/>
       <c r="AE7" s="7" t="str">
         <f>MID(AE$6,$P7,1)</f>
-        <v>Q</v>
-      </c>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-    </row>
-    <row r="8" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="17" t="s">
+        <v>F</v>
+      </c>
+      <c r="AF7" s="7" t="str">
+        <f>MID(AF$6,$P7,1)</f>
+        <v>M</v>
+      </c>
+      <c r="AG7" s="1">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+    </row>
+    <row r="8" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="13"/>
+      <c r="N8" s="13"/>
+      <c r="O8" s="13"/>
       <c r="P8" s="3">
         <v>2</v>
       </c>
@@ -942,79 +997,85 @@
         <v>2</v>
       </c>
       <c r="R8" s="2" cm="1">
-        <f t="array" aca="1" ref="R8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,R$5+1,1),OFFSET(R8,-1,-1),MIN(1+OFFSET(R8,0,-1),1+OFFSET(R8,-1,0),1+OFFSET(R8,-1,-1)))</f>
+        <f t="array" aca="1" ref="R8" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P8,0),OFFSET(R8,-1,-1),MIN(1+OFFSET(R8,-1,0),1+OFFSET(R8,0,-1),1+OFFSET(R8,-1,-1)))</f>
         <v>2</v>
       </c>
       <c r="S8" s="2" cm="1">
-        <f t="array" aca="1" ref="S8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,S$5+1,1),OFFSET(S8,-1,-1),MIN(1+OFFSET(S8,0,-1),1+OFFSET(S8,-1,0),1+OFFSET(S8,-1,-1)))</f>
+        <f t="array" aca="1" ref="S8" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P8,0),OFFSET(S8,-1,-1),MIN(1+OFFSET(S8,-1,0),1+OFFSET(S8,0,-1),1+OFFSET(S8,-1,-1)))</f>
+        <v>1</v>
+      </c>
+      <c r="T8" s="2" cm="1">
+        <f t="array" aca="1" ref="T8" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P8,0),OFFSET(T8,-1,-1),MIN(1+OFFSET(T8,-1,0),1+OFFSET(T8,0,-1),1+OFFSET(T8,-1,-1)))</f>
         <v>2</v>
       </c>
-      <c r="T8" s="2" cm="1">
-        <f t="array" aca="1" ref="T8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,T$5+1,1),OFFSET(T8,-1,-1),MIN(1+OFFSET(T8,0,-1),1+OFFSET(T8,-1,0),1+OFFSET(T8,-1,-1)))</f>
-        <v>2</v>
-      </c>
       <c r="U8" s="2" cm="1">
-        <f t="array" aca="1" ref="U8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,U$5+1,1),OFFSET(U8,-1,-1),MIN(1+OFFSET(U8,0,-1),1+OFFSET(U8,-1,0),1+OFFSET(U8,-1,-1)))</f>
+        <f t="array" aca="1" ref="U8" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P8,0),OFFSET(U8,-1,-1),MIN(1+OFFSET(U8,-1,0),1+OFFSET(U8,0,-1),1+OFFSET(U8,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="V8" s="2" cm="1">
-        <f t="array" aca="1" ref="V8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,V$5+1,1),OFFSET(V8,-1,-1),MIN(1+OFFSET(V8,0,-1),1+OFFSET(V8,-1,0),1+OFFSET(V8,-1,-1)))</f>
+        <f t="array" aca="1" ref="V8" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P8,0),OFFSET(V8,-1,-1),MIN(1+OFFSET(V8,-1,0),1+OFFSET(V8,0,-1),1+OFFSET(V8,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="W8" s="2" cm="1">
-        <f t="array" aca="1" ref="W8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,W$5+1,1),OFFSET(W8,-1,-1),MIN(1+OFFSET(W8,0,-1),1+OFFSET(W8,-1,0),1+OFFSET(W8,-1,-1)))</f>
+        <f t="array" aca="1" ref="W8" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P8,0),OFFSET(W8,-1,-1),MIN(1+OFFSET(W8,-1,0),1+OFFSET(W8,0,-1),1+OFFSET(W8,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="X8" s="2" cm="1">
-        <f t="array" aca="1" ref="X8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,X$5+1,1),OFFSET(X8,-1,-1),MIN(1+OFFSET(X8,0,-1),1+OFFSET(X8,-1,0),1+OFFSET(X8,-1,-1)))</f>
+        <f t="array" aca="1" ref="X8" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P8,0),OFFSET(X8,-1,-1),MIN(1+OFFSET(X8,-1,0),1+OFFSET(X8,0,-1),1+OFFSET(X8,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="Y8" s="2" cm="1">
-        <f t="array" aca="1" ref="Y8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y8,-1,-1),MIN(1+OFFSET(Y8,0,-1),1+OFFSET(Y8,-1,0),1+OFFSET(Y8,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y8" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P8,0),OFFSET(Y8,-1,-1),MIN(1+OFFSET(Y8,-1,0),1+OFFSET(Y8,0,-1),1+OFFSET(Y8,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="Z8" s="2" cm="1">
-        <f t="array" aca="1" ref="Z8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z8,-1,-1),MIN(1+OFFSET(Z8,0,-1),1+OFFSET(Z8,-1,0),1+OFFSET(Z8,-1,-1)))</f>
+        <f t="array" aca="1" ref="Z8" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P8,0),OFFSET(Z8,-1,-1),MIN(1+OFFSET(Z8,-1,0),1+OFFSET(Z8,0,-1),1+OFFSET(Z8,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="AA8" s="2" cm="1">
-        <f t="array" aca="1" ref="AA8" ca="1">IF(INDEX(X,$P8+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA8,-1,-1),MIN(1+OFFSET(AA8,0,-1),1+OFFSET(AA8,-1,0),1+OFFSET(AA8,-1,-1)))</f>
+        <f t="array" aca="1" ref="AA8" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P8,0),OFFSET(AA8,-1,-1),MIN(1+OFFSET(AA8,-1,0),1+OFFSET(AA8,0,-1),1+OFFSET(AA8,-1,-1)))</f>
         <v>9</v>
       </c>
-      <c r="AB8" s="1"/>
+      <c r="AB8" s="24"/>
       <c r="AC8" s="1"/>
-      <c r="AD8" s="7" t="str">
-        <f t="shared" ref="AD8:AE16" si="0">MID(AD$6,$P8,1)</f>
-        <v>B</v>
-      </c>
+      <c r="AD8" s="1"/>
       <c r="AE8" s="7" t="str">
+        <f t="shared" ref="AE7:AH16" si="0">MID(AE$6,$P8,1)</f>
+        <v>O</v>
+      </c>
+      <c r="AF8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-    </row>
-    <row r="9" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="17" t="s">
+        <v>O</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI8" s="1"/>
+      <c r="AJ8" s="1"/>
+    </row>
+    <row r="9" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="13"/>
+      <c r="N9" s="13"/>
+      <c r="O9" s="13"/>
       <c r="P9" s="3">
         <v>3</v>
       </c>
@@ -1022,75 +1083,81 @@
         <v>3</v>
       </c>
       <c r="R9" s="2" cm="1">
-        <f t="array" aca="1" ref="R9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,R$5+1,1),OFFSET(R9,-1,-1),MIN(1+OFFSET(R9,0,-1),1+OFFSET(R9,-1,0),1+OFFSET(R9,-1,-1)))</f>
+        <f t="array" aca="1" ref="R9" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P9,0),OFFSET(R9,-1,-1),MIN(1+OFFSET(R9,-1,0),1+OFFSET(R9,0,-1),1+OFFSET(R9,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="S9" s="2" cm="1">
-        <f t="array" aca="1" ref="S9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,S$5+1,1),OFFSET(S9,-1,-1),MIN(1+OFFSET(S9,0,-1),1+OFFSET(S9,-1,0),1+OFFSET(S9,-1,-1)))</f>
+        <f t="array" aca="1" ref="S9" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P9,0),OFFSET(S9,-1,-1),MIN(1+OFFSET(S9,-1,0),1+OFFSET(S9,0,-1),1+OFFSET(S9,-1,-1)))</f>
+        <v>2</v>
+      </c>
+      <c r="T9" s="2" cm="1">
+        <f t="array" aca="1" ref="T9" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P9,0),OFFSET(T9,-1,-1),MIN(1+OFFSET(T9,-1,0),1+OFFSET(T9,0,-1),1+OFFSET(T9,-1,-1)))</f>
+        <v>2</v>
+      </c>
+      <c r="U9" s="2" cm="1">
+        <f t="array" aca="1" ref="U9" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P9,0),OFFSET(U9,-1,-1),MIN(1+OFFSET(U9,-1,0),1+OFFSET(U9,0,-1),1+OFFSET(U9,-1,-1)))</f>
         <v>3</v>
       </c>
-      <c r="T9" s="2" cm="1">
-        <f t="array" aca="1" ref="T9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,T$5+1,1),OFFSET(T9,-1,-1),MIN(1+OFFSET(T9,0,-1),1+OFFSET(T9,-1,0),1+OFFSET(T9,-1,-1)))</f>
-        <v>2</v>
-      </c>
-      <c r="U9" s="2" cm="1">
-        <f t="array" aca="1" ref="U9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,U$5+1,1),OFFSET(U9,-1,-1),MIN(1+OFFSET(U9,0,-1),1+OFFSET(U9,-1,0),1+OFFSET(U9,-1,-1)))</f>
-        <v>3</v>
-      </c>
       <c r="V9" s="2" cm="1">
-        <f t="array" aca="1" ref="V9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,V$5+1,1),OFFSET(V9,-1,-1),MIN(1+OFFSET(V9,0,-1),1+OFFSET(V9,-1,0),1+OFFSET(V9,-1,-1)))</f>
+        <f t="array" aca="1" ref="V9" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P9,0),OFFSET(V9,-1,-1),MIN(1+OFFSET(V9,-1,0),1+OFFSET(V9,0,-1),1+OFFSET(V9,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="W9" s="2" cm="1">
-        <f t="array" aca="1" ref="W9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,W$5+1,1),OFFSET(W9,-1,-1),MIN(1+OFFSET(W9,0,-1),1+OFFSET(W9,-1,0),1+OFFSET(W9,-1,-1)))</f>
+        <f t="array" aca="1" ref="W9" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P9,0),OFFSET(W9,-1,-1),MIN(1+OFFSET(W9,-1,0),1+OFFSET(W9,0,-1),1+OFFSET(W9,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="X9" s="2" cm="1">
-        <f t="array" aca="1" ref="X9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,X$5+1,1),OFFSET(X9,-1,-1),MIN(1+OFFSET(X9,0,-1),1+OFFSET(X9,-1,0),1+OFFSET(X9,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="X9" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P9,0),OFFSET(X9,-1,-1),MIN(1+OFFSET(X9,-1,0),1+OFFSET(X9,0,-1),1+OFFSET(X9,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="Y9" s="2" cm="1">
-        <f t="array" aca="1" ref="Y9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y9,-1,-1),MIN(1+OFFSET(Y9,0,-1),1+OFFSET(Y9,-1,0),1+OFFSET(Y9,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="Y9" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P9,0),OFFSET(Y9,-1,-1),MIN(1+OFFSET(Y9,-1,0),1+OFFSET(Y9,0,-1),1+OFFSET(Y9,-1,-1)))</f>
+        <v>7</v>
       </c>
       <c r="Z9" s="2" cm="1">
-        <f t="array" aca="1" ref="Z9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z9,-1,-1),MIN(1+OFFSET(Z9,0,-1),1+OFFSET(Z9,-1,0),1+OFFSET(Z9,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="Z9" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P9,0),OFFSET(Z9,-1,-1),MIN(1+OFFSET(Z9,-1,0),1+OFFSET(Z9,0,-1),1+OFFSET(Z9,-1,-1)))</f>
+        <v>8</v>
       </c>
       <c r="AA9" s="2" cm="1">
-        <f t="array" aca="1" ref="AA9" ca="1">IF(INDEX(X,$P9+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA9,-1,-1),MIN(1+OFFSET(AA9,0,-1),1+OFFSET(AA9,-1,0),1+OFFSET(AA9,-1,-1)))</f>
-        <v>8</v>
-      </c>
-      <c r="AB9" s="1"/>
+        <f t="array" aca="1" ref="AA9" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P9,0),OFFSET(AA9,-1,-1),MIN(1+OFFSET(AA9,-1,0),1+OFFSET(AA9,0,-1),1+OFFSET(AA9,-1,-1)))</f>
+        <v>9</v>
+      </c>
+      <c r="AB9" s="24"/>
       <c r="AC9" s="1"/>
-      <c r="AD9" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>B</v>
-      </c>
+      <c r="AD9" s="1"/>
       <c r="AE9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
-      </c>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-    </row>
-    <row r="10" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="14"/>
+        <v>O</v>
+      </c>
+      <c r="AF9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>N</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AH9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+    </row>
+    <row r="10" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="13"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="13"/>
       <c r="P10" s="3">
         <v>4</v>
       </c>
@@ -1098,144 +1165,157 @@
         <v>4</v>
       </c>
       <c r="R10" s="2" cm="1">
-        <f t="array" aca="1" ref="R10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,R$5+1,1),OFFSET(R10,-1,-1),MIN(1+OFFSET(R10,0,-1),1+OFFSET(R10,-1,0),1+OFFSET(R10,-1,-1)))</f>
+        <f t="array" aca="1" ref="R10" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P10,0),OFFSET(R10,-1,-1),MIN(1+OFFSET(R10,-1,0),1+OFFSET(R10,0,-1),1+OFFSET(R10,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="S10" s="2" cm="1">
-        <f t="array" aca="1" ref="S10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,S$5+1,1),OFFSET(S10,-1,-1),MIN(1+OFFSET(S10,0,-1),1+OFFSET(S10,-1,0),1+OFFSET(S10,-1,-1)))</f>
-        <v>4</v>
+        <f t="array" aca="1" ref="S10" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P10,0),OFFSET(S10,-1,-1),MIN(1+OFFSET(S10,-1,0),1+OFFSET(S10,0,-1),1+OFFSET(S10,-1,-1)))</f>
+        <v>3</v>
       </c>
       <c r="T10" s="2" cm="1">
-        <f t="array" aca="1" ref="T10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,T$5+1,1),OFFSET(T10,-1,-1),MIN(1+OFFSET(T10,0,-1),1+OFFSET(T10,-1,0),1+OFFSET(T10,-1,-1)))</f>
+        <f t="array" aca="1" ref="T10" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P10,0),OFFSET(T10,-1,-1),MIN(1+OFFSET(T10,-1,0),1+OFFSET(T10,0,-1),1+OFFSET(T10,-1,-1)))</f>
         <v>3</v>
       </c>
       <c r="U10" s="2" cm="1">
-        <f t="array" aca="1" ref="U10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,U$5+1,1),OFFSET(U10,-1,-1),MIN(1+OFFSET(U10,0,-1),1+OFFSET(U10,-1,0),1+OFFSET(U10,-1,-1)))</f>
-        <v>2</v>
+        <f t="array" aca="1" ref="U10" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P10,0),OFFSET(U10,-1,-1),MIN(1+OFFSET(U10,-1,0),1+OFFSET(U10,0,-1),1+OFFSET(U10,-1,-1)))</f>
+        <v>3</v>
       </c>
       <c r="V10" s="2" cm="1">
-        <f t="array" aca="1" ref="V10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,V$5+1,1),OFFSET(V10,-1,-1),MIN(1+OFFSET(V10,0,-1),1+OFFSET(V10,-1,0),1+OFFSET(V10,-1,-1)))</f>
-        <v>3</v>
+        <f t="array" aca="1" ref="V10" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P10,0),OFFSET(V10,-1,-1),MIN(1+OFFSET(V10,-1,0),1+OFFSET(V10,0,-1),1+OFFSET(V10,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="W10" s="2" cm="1">
-        <f t="array" aca="1" ref="W10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,W$5+1,1),OFFSET(W10,-1,-1),MIN(1+OFFSET(W10,0,-1),1+OFFSET(W10,-1,0),1+OFFSET(W10,-1,-1)))</f>
-        <v>4</v>
+        <f t="array" aca="1" ref="W10" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P10,0),OFFSET(W10,-1,-1),MIN(1+OFFSET(W10,-1,0),1+OFFSET(W10,0,-1),1+OFFSET(W10,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="X10" s="2" cm="1">
-        <f t="array" aca="1" ref="X10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,X$5+1,1),OFFSET(X10,-1,-1),MIN(1+OFFSET(X10,0,-1),1+OFFSET(X10,-1,0),1+OFFSET(X10,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="X10" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P10,0),OFFSET(X10,-1,-1),MIN(1+OFFSET(X10,-1,0),1+OFFSET(X10,0,-1),1+OFFSET(X10,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="Y10" s="2" cm="1">
-        <f t="array" aca="1" ref="Y10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y10,-1,-1),MIN(1+OFFSET(Y10,0,-1),1+OFFSET(Y10,-1,0),1+OFFSET(Y10,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="Y10" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P10,0),OFFSET(Y10,-1,-1),MIN(1+OFFSET(Y10,-1,0),1+OFFSET(Y10,0,-1),1+OFFSET(Y10,-1,-1)))</f>
+        <v>7</v>
       </c>
       <c r="Z10" s="2" cm="1">
-        <f t="array" aca="1" ref="Z10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z10,-1,-1),MIN(1+OFFSET(Z10,0,-1),1+OFFSET(Z10,-1,0),1+OFFSET(Z10,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="Z10" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P10,0),OFFSET(Z10,-1,-1),MIN(1+OFFSET(Z10,-1,0),1+OFFSET(Z10,0,-1),1+OFFSET(Z10,-1,-1)))</f>
+        <v>8</v>
       </c>
       <c r="AA10" s="2" cm="1">
-        <f t="array" aca="1" ref="AA10" ca="1">IF(INDEX(X,$P10+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA10,-1,-1),MIN(1+OFFSET(AA10,0,-1),1+OFFSET(AA10,-1,0),1+OFFSET(AA10,-1,-1)))</f>
-        <v>8</v>
-      </c>
-      <c r="AB10" s="1"/>
+        <f t="array" aca="1" ref="AA10" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P10,0),OFFSET(AA10,-1,-1),MIN(1+OFFSET(AA10,-1,0),1+OFFSET(AA10,0,-1),1+OFFSET(AA10,-1,-1)))</f>
+        <v>9</v>
+      </c>
+      <c r="AB10" s="24"/>
       <c r="AC10" s="1"/>
-      <c r="AD10" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>C</v>
-      </c>
+      <c r="AD10" s="1"/>
       <c r="AE10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>C</v>
-      </c>
-      <c r="AF10" s="1"/>
-    </row>
-    <row r="11" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="14"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="14"/>
-      <c r="M11" s="14"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="14"/>
-      <c r="P11" s="3">
-        <v>5</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>5</v>
-      </c>
-      <c r="R11" s="2" cm="1">
-        <f t="array" aca="1" ref="R11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,R$5+1,1),OFFSET(R11,-1,-1),MIN(1+OFFSET(R11,0,-1),1+OFFSET(R11,-1,0),1+OFFSET(R11,-1,-1)))</f>
-        <v>5</v>
-      </c>
-      <c r="S11" s="2" cm="1">
-        <f t="array" aca="1" ref="S11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,S$5+1,1),OFFSET(S11,-1,-1),MIN(1+OFFSET(S11,0,-1),1+OFFSET(S11,-1,0),1+OFFSET(S11,-1,-1)))</f>
-        <v>5</v>
-      </c>
-      <c r="T11" s="2" cm="1">
-        <f t="array" aca="1" ref="T11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,T$5+1,1),OFFSET(T11,-1,-1),MIN(1+OFFSET(T11,0,-1),1+OFFSET(T11,-1,0),1+OFFSET(T11,-1,-1)))</f>
-        <v>4</v>
-      </c>
-      <c r="U11" s="2" cm="1">
-        <f t="array" aca="1" ref="U11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,U$5+1,1),OFFSET(U11,-1,-1),MIN(1+OFFSET(U11,0,-1),1+OFFSET(U11,-1,0),1+OFFSET(U11,-1,-1)))</f>
-        <v>3</v>
-      </c>
-      <c r="V11" s="2" cm="1">
-        <f t="array" aca="1" ref="V11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,V$5+1,1),OFFSET(V11,-1,-1),MIN(1+OFFSET(V11,0,-1),1+OFFSET(V11,-1,0),1+OFFSET(V11,-1,-1)))</f>
-        <v>3</v>
-      </c>
-      <c r="W11" s="2" cm="1">
-        <f t="array" aca="1" ref="W11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,W$5+1,1),OFFSET(W11,-1,-1),MIN(1+OFFSET(W11,0,-1),1+OFFSET(W11,-1,0),1+OFFSET(W11,-1,-1)))</f>
-        <v>4</v>
-      </c>
-      <c r="X11" s="2" cm="1">
-        <f t="array" aca="1" ref="X11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,X$5+1,1),OFFSET(X11,-1,-1),MIN(1+OFFSET(X11,0,-1),1+OFFSET(X11,-1,0),1+OFFSET(X11,-1,-1)))</f>
-        <v>5</v>
-      </c>
-      <c r="Y11" s="2" cm="1">
-        <f t="array" aca="1" ref="Y11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y11,-1,-1),MIN(1+OFFSET(Y11,0,-1),1+OFFSET(Y11,-1,0),1+OFFSET(Y11,-1,-1)))</f>
-        <v>5</v>
-      </c>
-      <c r="Z11" s="2" cm="1">
-        <f t="array" aca="1" ref="Z11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z11,-1,-1),MIN(1+OFFSET(Z11,0,-1),1+OFFSET(Z11,-1,0),1+OFFSET(Z11,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="AA11" s="2" cm="1">
-        <f t="array" aca="1" ref="AA11" ca="1">IF(INDEX(X,$P11+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA11,-1,-1),MIN(1+OFFSET(AA11,0,-1),1+OFFSET(AA11,-1,0),1+OFFSET(AA11,-1,-1)))</f>
-        <v>7</v>
-      </c>
-      <c r="AD11" s="7" t="str">
+        <v>D</v>
+      </c>
+      <c r="AF10" s="7" t="str">
         <f t="shared" si="0"/>
         <v>E</v>
       </c>
+      <c r="AG10" s="1">
+        <v>3</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="3">
+        <v>5</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>5</v>
+      </c>
+      <c r="R11" s="2" cm="1">
+        <f t="array" aca="1" ref="R11" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P11,0),OFFSET(R11,-1,-1),MIN(1+OFFSET(R11,-1,0),1+OFFSET(R11,0,-1),1+OFFSET(R11,-1,-1)))</f>
+        <v>5</v>
+      </c>
+      <c r="S11" s="2" cm="1">
+        <f t="array" aca="1" ref="S11" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P11,0),OFFSET(S11,-1,-1),MIN(1+OFFSET(S11,-1,0),1+OFFSET(S11,0,-1),1+OFFSET(S11,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="T11" s="2" cm="1">
+        <f t="array" aca="1" ref="T11" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P11,0),OFFSET(T11,-1,-1),MIN(1+OFFSET(T11,-1,0),1+OFFSET(T11,0,-1),1+OFFSET(T11,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="U11" s="2" cm="1">
+        <f t="array" aca="1" ref="U11" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P11,0),OFFSET(U11,-1,-1),MIN(1+OFFSET(U11,-1,0),1+OFFSET(U11,0,-1),1+OFFSET(U11,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="V11" s="2" cm="1">
+        <f t="array" aca="1" ref="V11" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P11,0),OFFSET(V11,-1,-1),MIN(1+OFFSET(V11,-1,0),1+OFFSET(V11,0,-1),1+OFFSET(V11,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="W11" s="2" cm="1">
+        <f t="array" aca="1" ref="W11" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P11,0),OFFSET(W11,-1,-1),MIN(1+OFFSET(W11,-1,0),1+OFFSET(W11,0,-1),1+OFFSET(W11,-1,-1)))</f>
+        <v>5</v>
+      </c>
+      <c r="X11" s="2" cm="1">
+        <f t="array" aca="1" ref="X11" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P11,0),OFFSET(X11,-1,-1),MIN(1+OFFSET(X11,-1,0),1+OFFSET(X11,0,-1),1+OFFSET(X11,-1,-1)))</f>
+        <v>6</v>
+      </c>
+      <c r="Y11" s="2" cm="1">
+        <f t="array" aca="1" ref="Y11" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P11,0),OFFSET(Y11,-1,-1),MIN(1+OFFSET(Y11,-1,0),1+OFFSET(Y11,0,-1),1+OFFSET(Y11,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="Z11" s="2" cm="1">
+        <f t="array" aca="1" ref="Z11" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P11,0),OFFSET(Z11,-1,-1),MIN(1+OFFSET(Z11,-1,0),1+OFFSET(Z11,0,-1),1+OFFSET(Z11,-1,-1)))</f>
+        <v>8</v>
+      </c>
+      <c r="AA11" s="2" cm="1">
+        <f t="array" aca="1" ref="AA11" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P11,0),OFFSET(AA11,-1,-1),MIN(1+OFFSET(AA11,-1,0),1+OFFSET(AA11,0,-1),1+OFFSET(AA11,-1,-1)))</f>
+        <v>9</v>
+      </c>
+      <c r="AB11" s="24"/>
       <c r="AE11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>D</v>
-      </c>
-    </row>
-    <row r="12" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+        <v/>
+      </c>
+      <c r="AF11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>Y</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>4</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="13"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13"/>
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="13"/>
       <c r="P12" s="3">
         <v>6</v>
       </c>
@@ -1243,70 +1323,77 @@
         <v>6</v>
       </c>
       <c r="R12" s="2" cm="1">
-        <f t="array" aca="1" ref="R12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,R$5+1,1),OFFSET(R12,-1,-1),MIN(1+OFFSET(R12,0,-1),1+OFFSET(R12,-1,0),1+OFFSET(R12,-1,-1)))</f>
+        <f t="array" aca="1" ref="R12" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P12,0),OFFSET(R12,-1,-1),MIN(1+OFFSET(R12,-1,0),1+OFFSET(R12,0,-1),1+OFFSET(R12,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="S12" s="2" cm="1">
-        <f t="array" aca="1" ref="S12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,S$5+1,1),OFFSET(S12,-1,-1),MIN(1+OFFSET(S12,0,-1),1+OFFSET(S12,-1,0),1+OFFSET(S12,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="S12" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P12,0),OFFSET(S12,-1,-1),MIN(1+OFFSET(S12,-1,0),1+OFFSET(S12,0,-1),1+OFFSET(S12,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="T12" s="2" cm="1">
-        <f t="array" aca="1" ref="T12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,T$5+1,1),OFFSET(T12,-1,-1),MIN(1+OFFSET(T12,0,-1),1+OFFSET(T12,-1,0),1+OFFSET(T12,-1,-1)))</f>
+        <f t="array" aca="1" ref="T12" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P12,0),OFFSET(T12,-1,-1),MIN(1+OFFSET(T12,-1,0),1+OFFSET(T12,0,-1),1+OFFSET(T12,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="U12" s="2" cm="1">
-        <f t="array" aca="1" ref="U12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,U$5+1,1),OFFSET(U12,-1,-1),MIN(1+OFFSET(U12,0,-1),1+OFFSET(U12,-1,0),1+OFFSET(U12,-1,-1)))</f>
-        <v>4</v>
+        <f t="array" aca="1" ref="U12" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P12,0),OFFSET(U12,-1,-1),MIN(1+OFFSET(U12,-1,0),1+OFFSET(U12,0,-1),1+OFFSET(U12,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="V12" s="2" cm="1">
-        <f t="array" aca="1" ref="V12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,V$5+1,1),OFFSET(V12,-1,-1),MIN(1+OFFSET(V12,0,-1),1+OFFSET(V12,-1,0),1+OFFSET(V12,-1,-1)))</f>
+        <f t="array" aca="1" ref="V12" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P12,0),OFFSET(V12,-1,-1),MIN(1+OFFSET(V12,-1,0),1+OFFSET(V12,0,-1),1+OFFSET(V12,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="W12" s="2" cm="1">
-        <f t="array" aca="1" ref="W12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,W$5+1,1),OFFSET(W12,-1,-1),MIN(1+OFFSET(W12,0,-1),1+OFFSET(W12,-1,0),1+OFFSET(W12,-1,-1)))</f>
+        <f t="array" aca="1" ref="W12" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P12,0),OFFSET(W12,-1,-1),MIN(1+OFFSET(W12,-1,0),1+OFFSET(W12,0,-1),1+OFFSET(W12,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="X12" s="2" cm="1">
-        <f t="array" aca="1" ref="X12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,X$5+1,1),OFFSET(X12,-1,-1),MIN(1+OFFSET(X12,0,-1),1+OFFSET(X12,-1,0),1+OFFSET(X12,-1,-1)))</f>
+        <f t="array" aca="1" ref="X12" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P12,0),OFFSET(X12,-1,-1),MIN(1+OFFSET(X12,-1,0),1+OFFSET(X12,0,-1),1+OFFSET(X12,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="Y12" s="2" cm="1">
-        <f t="array" aca="1" ref="Y12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y12,-1,-1),MIN(1+OFFSET(Y12,0,-1),1+OFFSET(Y12,-1,0),1+OFFSET(Y12,-1,-1)))</f>
+        <f t="array" aca="1" ref="Y12" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P12,0),OFFSET(Y12,-1,-1),MIN(1+OFFSET(Y12,-1,0),1+OFFSET(Y12,0,-1),1+OFFSET(Y12,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="Z12" s="2" cm="1">
-        <f t="array" aca="1" ref="Z12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z12,-1,-1),MIN(1+OFFSET(Z12,0,-1),1+OFFSET(Z12,-1,0),1+OFFSET(Z12,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="Z12" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P12,0),OFFSET(Z12,-1,-1),MIN(1+OFFSET(Z12,-1,0),1+OFFSET(Z12,0,-1),1+OFFSET(Z12,-1,-1)))</f>
+        <v>7</v>
       </c>
       <c r="AA12" s="2" cm="1">
-        <f t="array" aca="1" ref="AA12" ca="1">IF(INDEX(X,$P12+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA12,-1,-1),MIN(1+OFFSET(AA12,0,-1),1+OFFSET(AA12,-1,0),1+OFFSET(AA12,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="AD12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
+        <f t="array" aca="1" ref="AA12" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P12,0),OFFSET(AA12,-1,-1),MIN(1+OFFSET(AA12,-1,0),1+OFFSET(AA12,0,-1),1+OFFSET(AA12,-1,-1)))</f>
+        <v>8</v>
+      </c>
+      <c r="AB12" s="24"/>
       <c r="AE12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="13" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="14"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="14"/>
-      <c r="L13" s="14"/>
-      <c r="M13" s="14"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="14"/>
+        <v/>
+      </c>
+      <c r="AF12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG12" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
       <c r="P13" s="3">
         <v>7</v>
       </c>
@@ -1314,70 +1401,77 @@
         <v>7</v>
       </c>
       <c r="R13" s="2" cm="1">
-        <f t="array" aca="1" ref="R13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,R$5+1,1),OFFSET(R13,-1,-1),MIN(1+OFFSET(R13,0,-1),1+OFFSET(R13,-1,0),1+OFFSET(R13,-1,-1)))</f>
+        <f t="array" aca="1" ref="R13" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P13,0),OFFSET(R13,-1,-1),MIN(1+OFFSET(R13,-1,0),1+OFFSET(R13,0,-1),1+OFFSET(R13,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="S13" s="2" cm="1">
-        <f t="array" aca="1" ref="S13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,S$5+1,1),OFFSET(S13,-1,-1),MIN(1+OFFSET(S13,0,-1),1+OFFSET(S13,-1,0),1+OFFSET(S13,-1,-1)))</f>
+        <f t="array" aca="1" ref="S13" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P13,0),OFFSET(S13,-1,-1),MIN(1+OFFSET(S13,-1,0),1+OFFSET(S13,0,-1),1+OFFSET(S13,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="T13" s="2" cm="1">
-        <f t="array" aca="1" ref="T13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,T$5+1,1),OFFSET(T13,-1,-1),MIN(1+OFFSET(T13,0,-1),1+OFFSET(T13,-1,0),1+OFFSET(T13,-1,-1)))</f>
+        <f t="array" aca="1" ref="T13" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P13,0),OFFSET(T13,-1,-1),MIN(1+OFFSET(T13,-1,0),1+OFFSET(T13,0,-1),1+OFFSET(T13,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="U13" s="2" cm="1">
-        <f t="array" aca="1" ref="U13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,U$5+1,1),OFFSET(U13,-1,-1),MIN(1+OFFSET(U13,0,-1),1+OFFSET(U13,-1,0),1+OFFSET(U13,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="U13" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P13,0),OFFSET(U13,-1,-1),MIN(1+OFFSET(U13,-1,0),1+OFFSET(U13,0,-1),1+OFFSET(U13,-1,-1)))</f>
+        <v>6</v>
       </c>
       <c r="V13" s="2" cm="1">
-        <f t="array" aca="1" ref="V13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,V$5+1,1),OFFSET(V13,-1,-1),MIN(1+OFFSET(V13,0,-1),1+OFFSET(V13,-1,0),1+OFFSET(V13,-1,-1)))</f>
+        <f t="array" aca="1" ref="V13" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P13,0),OFFSET(V13,-1,-1),MIN(1+OFFSET(V13,-1,0),1+OFFSET(V13,0,-1),1+OFFSET(V13,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="W13" s="2" cm="1">
-        <f t="array" aca="1" ref="W13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,W$5+1,1),OFFSET(W13,-1,-1),MIN(1+OFFSET(W13,0,-1),1+OFFSET(W13,-1,0),1+OFFSET(W13,-1,-1)))</f>
+        <f t="array" aca="1" ref="W13" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P13,0),OFFSET(W13,-1,-1),MIN(1+OFFSET(W13,-1,0),1+OFFSET(W13,0,-1),1+OFFSET(W13,-1,-1)))</f>
         <v>4</v>
       </c>
       <c r="X13" s="2" cm="1">
-        <f t="array" aca="1" ref="X13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,X$5+1,1),OFFSET(X13,-1,-1),MIN(1+OFFSET(X13,0,-1),1+OFFSET(X13,-1,0),1+OFFSET(X13,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="X13" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P13,0),OFFSET(X13,-1,-1),MIN(1+OFFSET(X13,-1,0),1+OFFSET(X13,0,-1),1+OFFSET(X13,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="Y13" s="2" cm="1">
-        <f t="array" aca="1" ref="Y13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y13,-1,-1),MIN(1+OFFSET(Y13,0,-1),1+OFFSET(Y13,-1,0),1+OFFSET(Y13,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="Y13" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P13,0),OFFSET(Y13,-1,-1),MIN(1+OFFSET(Y13,-1,0),1+OFFSET(Y13,0,-1),1+OFFSET(Y13,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="Z13" s="2" cm="1">
-        <f t="array" aca="1" ref="Z13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z13,-1,-1),MIN(1+OFFSET(Z13,0,-1),1+OFFSET(Z13,-1,0),1+OFFSET(Z13,-1,-1)))</f>
+        <f t="array" aca="1" ref="Z13" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P13,0),OFFSET(Z13,-1,-1),MIN(1+OFFSET(Z13,-1,0),1+OFFSET(Z13,0,-1),1+OFFSET(Z13,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="AA13" s="2" cm="1">
-        <f t="array" aca="1" ref="AA13" ca="1">IF(INDEX(X,$P13+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA13,-1,-1),MIN(1+OFFSET(AA13,0,-1),1+OFFSET(AA13,-1,0),1+OFFSET(AA13,-1,-1)))</f>
-        <v>5</v>
-      </c>
-      <c r="AD13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
+        <f t="array" aca="1" ref="AA13" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P13,0),OFFSET(AA13,-1,-1),MIN(1+OFFSET(AA13,-1,0),1+OFFSET(AA13,0,-1),1+OFFSET(AA13,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="AB13" s="24"/>
       <c r="AE13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>B</v>
-      </c>
-    </row>
-    <row r="14" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="14"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
+        <v/>
+      </c>
+      <c r="AF13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG13" s="1">
+        <v>6</v>
+      </c>
+      <c r="AH13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
+      <c r="N14" s="13"/>
+      <c r="O14" s="13"/>
       <c r="P14" s="3">
         <v>8</v>
       </c>
@@ -1385,154 +1479,206 @@
         <v>8</v>
       </c>
       <c r="R14" s="2" cm="1">
-        <f t="array" aca="1" ref="R14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,R$5+1,1),OFFSET(R14,-1,-1),MIN(1+OFFSET(R14,0,-1),1+OFFSET(R14,-1,0),1+OFFSET(R14,-1,-1)))</f>
+        <f t="array" aca="1" ref="R14" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P14,0),OFFSET(R14,-1,-1),MIN(1+OFFSET(R14,-1,0),1+OFFSET(R14,0,-1),1+OFFSET(R14,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="S14" s="2" cm="1">
-        <f t="array" aca="1" ref="S14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,S$5+1,1),OFFSET(S14,-1,-1),MIN(1+OFFSET(S14,0,-1),1+OFFSET(S14,-1,0),1+OFFSET(S14,-1,-1)))</f>
+        <f t="array" aca="1" ref="S14" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P14,0),OFFSET(S14,-1,-1),MIN(1+OFFSET(S14,-1,0),1+OFFSET(S14,0,-1),1+OFFSET(S14,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="T14" s="2" cm="1">
-        <f t="array" aca="1" ref="T14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,T$5+1,1),OFFSET(T14,-1,-1),MIN(1+OFFSET(T14,0,-1),1+OFFSET(T14,-1,0),1+OFFSET(T14,-1,-1)))</f>
+        <f t="array" aca="1" ref="T14" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P14,0),OFFSET(T14,-1,-1),MIN(1+OFFSET(T14,-1,0),1+OFFSET(T14,0,-1),1+OFFSET(T14,-1,-1)))</f>
         <v>7</v>
       </c>
       <c r="U14" s="2" cm="1">
-        <f t="array" aca="1" ref="U14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,U$5+1,1),OFFSET(U14,-1,-1),MIN(1+OFFSET(U14,0,-1),1+OFFSET(U14,-1,0),1+OFFSET(U14,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="U14" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P14,0),OFFSET(U14,-1,-1),MIN(1+OFFSET(U14,-1,0),1+OFFSET(U14,0,-1),1+OFFSET(U14,-1,-1)))</f>
+        <v>7</v>
       </c>
       <c r="V14" s="2" cm="1">
-        <f t="array" aca="1" ref="V14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,V$5+1,1),OFFSET(V14,-1,-1),MIN(1+OFFSET(V14,0,-1),1+OFFSET(V14,-1,0),1+OFFSET(V14,-1,-1)))</f>
+        <f t="array" aca="1" ref="V14" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P14,0),OFFSET(V14,-1,-1),MIN(1+OFFSET(V14,-1,0),1+OFFSET(V14,0,-1),1+OFFSET(V14,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="W14" s="2" cm="1">
-        <f t="array" aca="1" ref="W14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,W$5+1,1),OFFSET(W14,-1,-1),MIN(1+OFFSET(W14,0,-1),1+OFFSET(W14,-1,0),1+OFFSET(W14,-1,-1)))</f>
+        <f t="array" aca="1" ref="W14" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P14,0),OFFSET(W14,-1,-1),MIN(1+OFFSET(W14,-1,0),1+OFFSET(W14,0,-1),1+OFFSET(W14,-1,-1)))</f>
         <v>5</v>
       </c>
       <c r="X14" s="2" cm="1">
-        <f t="array" aca="1" ref="X14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,X$5+1,1),OFFSET(X14,-1,-1),MIN(1+OFFSET(X14,0,-1),1+OFFSET(X14,-1,0),1+OFFSET(X14,-1,-1)))</f>
-        <v>5</v>
+        <f t="array" aca="1" ref="X14" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P14,0),OFFSET(X14,-1,-1),MIN(1+OFFSET(X14,-1,0),1+OFFSET(X14,0,-1),1+OFFSET(X14,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="Y14" s="2" cm="1">
-        <f t="array" aca="1" ref="Y14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y14,-1,-1),MIN(1+OFFSET(Y14,0,-1),1+OFFSET(Y14,-1,0),1+OFFSET(Y14,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="Y14" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P14,0),OFFSET(Y14,-1,-1),MIN(1+OFFSET(Y14,-1,0),1+OFFSET(Y14,0,-1),1+OFFSET(Y14,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="Z14" s="2" cm="1">
-        <f t="array" aca="1" ref="Z14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z14,-1,-1),MIN(1+OFFSET(Z14,0,-1),1+OFFSET(Z14,-1,0),1+OFFSET(Z14,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="Z14" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P14,0),OFFSET(Z14,-1,-1),MIN(1+OFFSET(Z14,-1,0),1+OFFSET(Z14,0,-1),1+OFFSET(Z14,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="AA14" s="2" cm="1">
-        <f t="array" aca="1" ref="AA14" ca="1">IF(INDEX(X,$P14+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA14,-1,-1),MIN(1+OFFSET(AA14,0,-1),1+OFFSET(AA14,-1,0),1+OFFSET(AA14,-1,-1)))</f>
-        <v>6</v>
-      </c>
-      <c r="AD14" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>T</v>
-      </c>
+        <f t="array" aca="1" ref="AA14" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P14,0),OFFSET(AA14,-1,-1),MIN(1+OFFSET(AA14,-1,0),1+OFFSET(AA14,0,-1),1+OFFSET(AA14,-1,-1)))</f>
+        <v>6</v>
+      </c>
+      <c r="AB14" s="24"/>
       <c r="AE14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>E</v>
-      </c>
-    </row>
-    <row r="15" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="14"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="14"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="14"/>
+        <v/>
+      </c>
+      <c r="AF14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG14" s="1">
+        <v>7</v>
+      </c>
+      <c r="AH14" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="13"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="13"/>
+      <c r="N15" s="13"/>
+      <c r="O15" s="13"/>
       <c r="P15" s="3">
         <v>9</v>
       </c>
-      <c r="Q15" s="2" cm="1">
-        <f t="array" aca="1" ref="Q15" ca="1">IF(INDEX(X,Q$5+1,1)=INDEX(Y,$P15+1,1),OFFSET(Q15,-1,-1),MIN(1+OFFSET(Q15,0,-1),1+OFFSET(Q15,-1,0),1+OFFSET(Q15,-1,-1)))</f>
+      <c r="Q15" s="2">
         <v>9</v>
       </c>
       <c r="R15" s="2" cm="1">
-        <f t="array" aca="1" ref="R15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,R$5+1,1),OFFSET(R15,-1,-1),MIN(1+OFFSET(R15,0,-1),1+OFFSET(R15,-1,0),1+OFFSET(R15,-1,-1)))</f>
+        <f t="array" aca="1" ref="R15" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P15,0),OFFSET(R15,-1,-1),MIN(1+OFFSET(R15,-1,0),1+OFFSET(R15,0,-1),1+OFFSET(R15,-1,-1)))</f>
         <v>9</v>
       </c>
       <c r="S15" s="2" cm="1">
-        <f t="array" aca="1" ref="S15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,S$5+1,1),OFFSET(S15,-1,-1),MIN(1+OFFSET(S15,0,-1),1+OFFSET(S15,-1,0),1+OFFSET(S15,-1,-1)))</f>
+        <f t="array" aca="1" ref="S15" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P15,0),OFFSET(S15,-1,-1),MIN(1+OFFSET(S15,-1,0),1+OFFSET(S15,0,-1),1+OFFSET(S15,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="T15" s="2" cm="1">
-        <f t="array" aca="1" ref="T15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,T$5+1,1),OFFSET(T15,-1,-1),MIN(1+OFFSET(T15,0,-1),1+OFFSET(T15,-1,0),1+OFFSET(T15,-1,-1)))</f>
+        <f t="array" aca="1" ref="T15" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P15,0),OFFSET(T15,-1,-1),MIN(1+OFFSET(T15,-1,0),1+OFFSET(T15,0,-1),1+OFFSET(T15,-1,-1)))</f>
         <v>8</v>
       </c>
       <c r="U15" s="2" cm="1">
-        <f t="array" aca="1" ref="U15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,U$5+1,1),OFFSET(U15,-1,-1),MIN(1+OFFSET(U15,0,-1),1+OFFSET(U15,-1,0),1+OFFSET(U15,-1,-1)))</f>
+        <f t="array" aca="1" ref="U15" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P15,0),OFFSET(U15,-1,-1),MIN(1+OFFSET(U15,-1,0),1+OFFSET(U15,0,-1),1+OFFSET(U15,-1,-1)))</f>
+        <v>8</v>
+      </c>
+      <c r="V15" s="2" cm="1">
+        <f t="array" aca="1" ref="V15" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P15,0),OFFSET(V15,-1,-1),MIN(1+OFFSET(V15,-1,0),1+OFFSET(V15,0,-1),1+OFFSET(V15,-1,-1)))</f>
         <v>7</v>
       </c>
-      <c r="V15" s="2" cm="1">
-        <f t="array" aca="1" ref="V15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,V$5+1,1),OFFSET(V15,-1,-1),MIN(1+OFFSET(V15,0,-1),1+OFFSET(V15,-1,0),1+OFFSET(V15,-1,-1)))</f>
-        <v>7</v>
-      </c>
       <c r="W15" s="2" cm="1">
-        <f t="array" aca="1" ref="W15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,W$5+1,1),OFFSET(W15,-1,-1),MIN(1+OFFSET(W15,0,-1),1+OFFSET(W15,-1,0),1+OFFSET(W15,-1,-1)))</f>
+        <f t="array" aca="1" ref="W15" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P15,0),OFFSET(W15,-1,-1),MIN(1+OFFSET(W15,-1,0),1+OFFSET(W15,0,-1),1+OFFSET(W15,-1,-1)))</f>
         <v>6</v>
       </c>
       <c r="X15" s="2" cm="1">
-        <f t="array" aca="1" ref="X15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,X$5+1,1),OFFSET(X15,-1,-1),MIN(1+OFFSET(X15,0,-1),1+OFFSET(X15,-1,0),1+OFFSET(X15,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="X15" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P15,0),OFFSET(X15,-1,-1),MIN(1+OFFSET(X15,-1,0),1+OFFSET(X15,0,-1),1+OFFSET(X15,-1,-1)))</f>
+        <v>5</v>
       </c>
       <c r="Y15" s="2" cm="1">
-        <f t="array" aca="1" ref="Y15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,Y$5+1,1),OFFSET(Y15,-1,-1),MIN(1+OFFSET(Y15,0,-1),1+OFFSET(Y15,-1,0),1+OFFSET(Y15,-1,-1)))</f>
-        <v>6</v>
+        <f t="array" aca="1" ref="Y15" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P15,0),OFFSET(Y15,-1,-1),MIN(1+OFFSET(Y15,-1,0),1+OFFSET(Y15,0,-1),1+OFFSET(Y15,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="Z15" s="2" cm="1">
-        <f t="array" aca="1" ref="Z15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,Z$5+1,1),OFFSET(Z15,-1,-1),MIN(1+OFFSET(Z15,0,-1),1+OFFSET(Z15,-1,0),1+OFFSET(Z15,-1,-1)))</f>
-        <v>7</v>
+        <f t="array" aca="1" ref="Z15" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P15,0),OFFSET(Z15,-1,-1),MIN(1+OFFSET(Z15,-1,0),1+OFFSET(Z15,0,-1),1+OFFSET(Z15,-1,-1)))</f>
+        <v>4</v>
       </c>
       <c r="AA15" s="2" cm="1">
-        <f t="array" aca="1" ref="AA15" ca="1">IF(INDEX(X,$P15+1,1)=INDEX(Y,AA$5+1,1),OFFSET(AA15,-1,-1),MIN(1+OFFSET(AA15,0,-1),1+OFFSET(AA15,-1,0),1+OFFSET(AA15,-1,-1)))</f>
-        <v>7</v>
-      </c>
-      <c r="AD15" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>Z</v>
-      </c>
+        <f t="array" aca="1" ref="AA15" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P15,0),OFFSET(AA15,-1,-1),MIN(1+OFFSET(AA15,-1,0),1+OFFSET(AA15,0,-1),1+OFFSET(AA15,-1,-1)))</f>
+        <v>5</v>
+      </c>
+      <c r="AB15" s="24"/>
       <c r="AE15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="16" spans="1:34" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v/>
+      </c>
+      <c r="AF15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="AG15" s="1">
+        <v>8</v>
+      </c>
+      <c r="AH15" t="s">
+        <v>28</v>
+      </c>
+      <c r="AJ15" s="6"/>
+    </row>
+    <row r="16" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O16" s="10" t="s">
-        <v>25</v>
+        <v>46</v>
       </c>
       <c r="P16" s="3">
         <v>10</v>
       </c>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="2"/>
-      <c r="U16" s="2"/>
-      <c r="V16" s="2"/>
-      <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="2"/>
-      <c r="Z16" s="2"/>
-      <c r="AA16" s="2"/>
-      <c r="AD16" s="7" t="str">
+      <c r="Q16" s="2">
+        <v>10</v>
+      </c>
+      <c r="R16" s="2" cm="1">
+        <f t="array" aca="1" ref="R16" ca="1">IF(INDEX(X,R$5,0)=INDEX(Y,$P16,0),OFFSET(R16,-1,-1),MIN(1+OFFSET(R16,-1,0),1+OFFSET(R16,0,-1),1+OFFSET(R16,-1,-1)))</f>
+        <v>10</v>
+      </c>
+      <c r="S16" s="2" cm="1">
+        <f t="array" aca="1" ref="S16" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P16,0),OFFSET(S16,-1,-1),MIN(1+OFFSET(S16,-1,0),1+OFFSET(S16,0,-1),1+OFFSET(S16,-1,-1)))</f>
+        <v>9</v>
+      </c>
+      <c r="T16" s="2" cm="1">
+        <f t="array" aca="1" ref="T16" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P16,0),OFFSET(T16,-1,-1),MIN(1+OFFSET(T16,-1,0),1+OFFSET(T16,0,-1),1+OFFSET(T16,-1,-1)))</f>
+        <v>9</v>
+      </c>
+      <c r="U16" s="2" cm="1">
+        <f t="array" aca="1" ref="U16" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P16,0),OFFSET(U16,-1,-1),MIN(1+OFFSET(U16,-1,0),1+OFFSET(U16,0,-1),1+OFFSET(U16,-1,-1)))</f>
+        <v>9</v>
+      </c>
+      <c r="V16" s="2" cm="1">
+        <f t="array" aca="1" ref="V16" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P16,0),OFFSET(V16,-1,-1),MIN(1+OFFSET(V16,-1,0),1+OFFSET(V16,0,-1),1+OFFSET(V16,-1,-1)))</f>
+        <v>8</v>
+      </c>
+      <c r="W16" s="2" cm="1">
+        <f t="array" aca="1" ref="W16" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P16,0),OFFSET(W16,-1,-1),MIN(1+OFFSET(W16,-1,0),1+OFFSET(W16,0,-1),1+OFFSET(W16,-1,-1)))</f>
+        <v>7</v>
+      </c>
+      <c r="X16" s="2" cm="1">
+        <f t="array" aca="1" ref="X16" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P16,0),OFFSET(X16,-1,-1),MIN(1+OFFSET(X16,-1,0),1+OFFSET(X16,0,-1),1+OFFSET(X16,-1,-1)))</f>
+        <v>6</v>
+      </c>
+      <c r="Y16" s="2" cm="1">
+        <f t="array" aca="1" ref="Y16" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P16,0),OFFSET(Y16,-1,-1),MIN(1+OFFSET(Y16,-1,0),1+OFFSET(Y16,0,-1),1+OFFSET(Y16,-1,-1)))</f>
+        <v>5</v>
+      </c>
+      <c r="Z16" s="2" cm="1">
+        <f t="array" aca="1" ref="Z16" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P16,0),OFFSET(Z16,-1,-1),MIN(1+OFFSET(Z16,-1,0),1+OFFSET(Z16,0,-1),1+OFFSET(Z16,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="AA16" s="2" cm="1">
+        <f t="array" aca="1" ref="AA16" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P16,0),OFFSET(AA16,-1,-1),MIN(1+OFFSET(AA16,-1,0),1+OFFSET(AA16,0,-1),1+OFFSET(AA16,-1,-1)))</f>
+        <v>4</v>
+      </c>
+      <c r="AB16" s="24"/>
+      <c r="AE16" s="7" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE16" s="7" t="str">
+      <c r="AF16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="17" spans="16:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+        <v/>
+      </c>
+      <c r="AG16" s="1">
+        <v>9</v>
+      </c>
+      <c r="AI16" s="6"/>
+      <c r="AJ16" s="6"/>
+    </row>
+    <row r="17" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="P17" s="6"/>
       <c r="Q17" s="9"/>
       <c r="R17" s="9"/>
@@ -1545,28 +1691,92 @@
       <c r="Y17" s="9"/>
       <c r="Z17" s="9"/>
       <c r="AA17" s="9"/>
-    </row>
-    <row r="18" spans="16:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="8">
-        <f>COUNTIFS(AD$7:AD$16,"?")</f>
-        <v>9</v>
-      </c>
+      <c r="AB17" s="9"/>
+      <c r="AG17" s="1">
+        <v>10</v>
+      </c>
+      <c r="AI17" s="6"/>
+      <c r="AJ17" s="6"/>
+    </row>
+    <row r="18" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AD18" s="6"/>
       <c r="AE18" s="8">
         <f>COUNTIFS(AE$7:AE$16,"?")</f>
-        <v>10</v>
-      </c>
-      <c r="AF18" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="AF18" s="8">
+        <f>COUNTIFS(AF$7:AF$16,"?")</f>
+        <v>5</v>
+      </c>
+      <c r="AG18" s="11" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE20" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF20" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG20" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH20" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE21" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF21" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH21" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE22" s="18" t="str">
+        <f>AF21</f>
+        <v>PBBCEFATZAF</v>
+      </c>
+      <c r="AF22" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="AG22" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="AH22" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="AE23" s="18" t="str">
+        <f>AF22</f>
+        <v>PBBCEFATAF</v>
+      </c>
+      <c r="AF23" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG23" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH23" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AD4:AE4"/>
+    <mergeCell ref="AE4:AF4"/>
   </mergeCells>
-  <conditionalFormatting sqref="Q6:AA16">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND($P6=$AD$18,Q$5=$AE$18)</formula>
+  <conditionalFormatting sqref="Q6:AB16">
+    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+      <formula>AND($P6=$AF$18,Q$5=$AE$18)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Begin to code for Burglary problem
</commit_message>
<xml_diff>
--- a/DynamicPro/editDistance/editDistance.xlsx
+++ b/DynamicPro/editDistance/editDistance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/khoikhang/Documents/SWCPT/DynamicPro/editDistance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86350BEF-CF11-C343-B49C-E43BBCD40FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA9BBC8-61BB-5A4E-AEE0-2EFE1F15FE06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="500" windowWidth="27560" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="47">
   <si>
     <t>B2</t>
   </si>
@@ -138,10 +138,7 @@
     <t>PBBCEFATZ</t>
   </si>
   <si>
-    <t>FOOD</t>
-  </si>
-  <si>
-    <t>MONEY</t>
+    <t>QABCDABEFA</t>
   </si>
   <si>
     <t>E</t>
@@ -634,8 +631,8 @@
   </sheetPr>
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J4" zoomScale="125" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="J3" zoomScale="125" workbookViewId="0">
+      <selection activeCell="AC24" sqref="AC24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -645,8 +642,9 @@
     <col min="3" max="3" width="3.5" customWidth="1"/>
     <col min="4" max="13" width="3.6640625" customWidth="1"/>
     <col min="14" max="14" width="4.1640625" customWidth="1"/>
-    <col min="15" max="26" width="5" customWidth="1"/>
-    <col min="27" max="28" width="7.5" customWidth="1"/>
+    <col min="15" max="15" width="5" customWidth="1"/>
+    <col min="16" max="27" width="4.1640625" customWidth="1"/>
+    <col min="28" max="28" width="7.5" customWidth="1"/>
     <col min="29" max="29" width="6" customWidth="1"/>
     <col min="30" max="30" width="6.33203125" customWidth="1"/>
     <col min="31" max="32" width="13.6640625" style="18" bestFit="1" customWidth="1"/>
@@ -747,11 +745,15 @@
         <v>3</v>
       </c>
       <c r="AF4" s="21"/>
-      <c r="AG4" s="6"/>
-      <c r="AH4" s="6"/>
+      <c r="AG4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH4" s="22" t="s">
+        <v>24</v>
+      </c>
       <c r="AI4" s="6"/>
     </row>
-    <row r="5" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>9</v>
       </c>
@@ -805,7 +807,7 @@
       </c>
       <c r="AB5" s="23"/>
       <c r="AC5" s="26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AD5" s="1"/>
       <c r="AE5" s="7" t="s">
@@ -818,7 +820,7 @@
       <c r="AH5" s="6"/>
       <c r="AI5" s="6"/>
     </row>
-    <row r="6" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="16" t="s">
         <v>15</v>
       </c>
@@ -876,15 +878,15 @@
       </c>
       <c r="AB6" s="24"/>
       <c r="AE6" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF6" s="22" t="s">
         <v>24</v>
-      </c>
-      <c r="AF6" s="22" t="s">
-        <v>25</v>
       </c>
       <c r="AG6" s="7"/>
       <c r="AH6" s="19"/>
     </row>
-    <row r="7" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -955,22 +957,22 @@
       <c r="AD7" s="1"/>
       <c r="AE7" s="7" t="str">
         <f>MID(AE$6,$P7,1)</f>
-        <v>F</v>
+        <v>P</v>
       </c>
       <c r="AF7" s="7" t="str">
         <f>MID(AF$6,$P7,1)</f>
-        <v>M</v>
+        <v>Q</v>
       </c>
       <c r="AG7" s="1">
         <v>0</v>
       </c>
       <c r="AH7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>12</v>
       </c>
@@ -1002,23 +1004,23 @@
       </c>
       <c r="S8" s="2" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">IF(INDEX(X,S$5,0)=INDEX(Y,$P8,0),OFFSET(S8,-1,-1),MIN(1+OFFSET(S8,-1,0),1+OFFSET(S8,0,-1),1+OFFSET(S8,-1,-1)))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T8" s="2" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P8,0),OFFSET(T8,-1,-1),MIN(1+OFFSET(T8,-1,0),1+OFFSET(T8,0,-1),1+OFFSET(T8,-1,-1)))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U8" s="2" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P8,0),OFFSET(U8,-1,-1),MIN(1+OFFSET(U8,-1,0),1+OFFSET(U8,0,-1),1+OFFSET(U8,-1,-1)))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="V8" s="2" cm="1">
         <f t="array" aca="1" ref="V8" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P8,0),OFFSET(V8,-1,-1),MIN(1+OFFSET(V8,-1,0),1+OFFSET(V8,0,-1),1+OFFSET(V8,-1,-1)))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W8" s="2" cm="1">
         <f t="array" aca="1" ref="W8" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P8,0),OFFSET(W8,-1,-1),MIN(1+OFFSET(W8,-1,0),1+OFFSET(W8,0,-1),1+OFFSET(W8,-1,-1)))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X8" s="2" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P8,0),OFFSET(X8,-1,-1),MIN(1+OFFSET(X8,-1,0),1+OFFSET(X8,0,-1),1+OFFSET(X8,-1,-1)))</f>
@@ -1041,22 +1043,22 @@
       <c r="AD8" s="1"/>
       <c r="AE8" s="7" t="str">
         <f t="shared" ref="AE7:AH16" si="0">MID(AE$6,$P8,1)</f>
-        <v>O</v>
+        <v>B</v>
       </c>
       <c r="AF8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>O</v>
+        <v>A</v>
       </c>
       <c r="AG8" s="1">
         <v>1</v>
       </c>
       <c r="AH8" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI8" s="1"/>
       <c r="AJ8" s="1"/>
     </row>
-    <row r="9" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
@@ -1127,22 +1129,22 @@
       <c r="AD9" s="1"/>
       <c r="AE9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>O</v>
+        <v>B</v>
       </c>
       <c r="AF9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>N</v>
+        <v>B</v>
       </c>
       <c r="AG9" s="1">
         <v>2</v>
       </c>
       <c r="AH9" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AI9" s="1"/>
       <c r="AJ9" s="1"/>
     </row>
-    <row r="10" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="13"/>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
@@ -1178,51 +1180,51 @@
       </c>
       <c r="U10" s="2" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P10,0),OFFSET(U10,-1,-1),MIN(1+OFFSET(U10,-1,0),1+OFFSET(U10,0,-1),1+OFFSET(U10,-1,-1)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V10" s="2" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P10,0),OFFSET(V10,-1,-1),MIN(1+OFFSET(V10,-1,0),1+OFFSET(V10,0,-1),1+OFFSET(V10,-1,-1)))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W10" s="2" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P10,0),OFFSET(W10,-1,-1),MIN(1+OFFSET(W10,-1,0),1+OFFSET(W10,0,-1),1+OFFSET(W10,-1,-1)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X10" s="2" cm="1">
         <f t="array" aca="1" ref="X10" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P10,0),OFFSET(X10,-1,-1),MIN(1+OFFSET(X10,-1,0),1+OFFSET(X10,0,-1),1+OFFSET(X10,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y10" s="2" cm="1">
         <f t="array" aca="1" ref="Y10" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P10,0),OFFSET(Y10,-1,-1),MIN(1+OFFSET(Y10,-1,0),1+OFFSET(Y10,0,-1),1+OFFSET(Y10,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z10" s="2" cm="1">
         <f t="array" aca="1" ref="Z10" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P10,0),OFFSET(Z10,-1,-1),MIN(1+OFFSET(Z10,-1,0),1+OFFSET(Z10,0,-1),1+OFFSET(Z10,-1,-1)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA10" s="2" cm="1">
         <f t="array" aca="1" ref="AA10" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P10,0),OFFSET(AA10,-1,-1),MIN(1+OFFSET(AA10,-1,0),1+OFFSET(AA10,0,-1),1+OFFSET(AA10,-1,-1)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB10" s="24"/>
       <c r="AC10" s="1"/>
       <c r="AD10" s="1"/>
       <c r="AE10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="AF10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>E</v>
+        <v>C</v>
       </c>
       <c r="AG10" s="1">
         <v>3</v>
       </c>
       <c r="AH10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1258,49 +1260,49 @@
       </c>
       <c r="U11" s="2" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P11,0),OFFSET(U11,-1,-1),MIN(1+OFFSET(U11,-1,0),1+OFFSET(U11,0,-1),1+OFFSET(U11,-1,-1)))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="V11" s="2" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P11,0),OFFSET(V11,-1,-1),MIN(1+OFFSET(V11,-1,0),1+OFFSET(V11,0,-1),1+OFFSET(V11,-1,-1)))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="W11" s="2" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P11,0),OFFSET(W11,-1,-1),MIN(1+OFFSET(W11,-1,0),1+OFFSET(W11,0,-1),1+OFFSET(W11,-1,-1)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="X11" s="2" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P11,0),OFFSET(X11,-1,-1),MIN(1+OFFSET(X11,-1,0),1+OFFSET(X11,0,-1),1+OFFSET(X11,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="2" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P11,0),OFFSET(Y11,-1,-1),MIN(1+OFFSET(Y11,-1,0),1+OFFSET(Y11,0,-1),1+OFFSET(Y11,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z11" s="2" cm="1">
         <f t="array" aca="1" ref="Z11" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P11,0),OFFSET(Z11,-1,-1),MIN(1+OFFSET(Z11,-1,0),1+OFFSET(Z11,0,-1),1+OFFSET(Z11,-1,-1)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AA11" s="2" cm="1">
         <f t="array" aca="1" ref="AA11" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P11,0),OFFSET(AA11,-1,-1),MIN(1+OFFSET(AA11,-1,0),1+OFFSET(AA11,0,-1),1+OFFSET(AA11,-1,-1)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AB11" s="24"/>
       <c r="AE11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>E</v>
       </c>
       <c r="AF11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>Y</v>
+        <v>D</v>
       </c>
       <c r="AG11" s="1">
         <v>4</v>
       </c>
       <c r="AH11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="13"/>
@@ -1336,7 +1338,7 @@
       </c>
       <c r="U12" s="2" cm="1">
         <f t="array" aca="1" ref="U12" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P12,0),OFFSET(U12,-1,-1),MIN(1+OFFSET(U12,-1,0),1+OFFSET(U12,0,-1),1+OFFSET(U12,-1,-1)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="V12" s="2" cm="1">
         <f t="array" aca="1" ref="V12" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P12,0),OFFSET(V12,-1,-1),MIN(1+OFFSET(V12,-1,0),1+OFFSET(V12,0,-1),1+OFFSET(V12,-1,-1)))</f>
@@ -1348,37 +1350,37 @@
       </c>
       <c r="X12" s="2" cm="1">
         <f t="array" aca="1" ref="X12" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P12,0),OFFSET(X12,-1,-1),MIN(1+OFFSET(X12,-1,0),1+OFFSET(X12,0,-1),1+OFFSET(X12,-1,-1)))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y12" s="2" cm="1">
         <f t="array" aca="1" ref="Y12" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P12,0),OFFSET(Y12,-1,-1),MIN(1+OFFSET(Y12,-1,0),1+OFFSET(Y12,0,-1),1+OFFSET(Y12,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Z12" s="2" cm="1">
         <f t="array" aca="1" ref="Z12" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P12,0),OFFSET(Z12,-1,-1),MIN(1+OFFSET(Z12,-1,0),1+OFFSET(Z12,0,-1),1+OFFSET(Z12,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AA12" s="2" cm="1">
         <f t="array" aca="1" ref="AA12" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P12,0),OFFSET(AA12,-1,-1),MIN(1+OFFSET(AA12,-1,0),1+OFFSET(AA12,0,-1),1+OFFSET(AA12,-1,-1)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AB12" s="24"/>
       <c r="AE12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>F</v>
       </c>
       <c r="AF12" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>A</v>
       </c>
       <c r="AG12" s="1">
         <v>5</v>
       </c>
       <c r="AH12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1410,11 +1412,11 @@
       </c>
       <c r="T13" s="2" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P13,0),OFFSET(T13,-1,-1),MIN(1+OFFSET(T13,-1,0),1+OFFSET(T13,0,-1),1+OFFSET(T13,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U13" s="2" cm="1">
         <f t="array" aca="1" ref="U13" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P13,0),OFFSET(U13,-1,-1),MIN(1+OFFSET(U13,-1,0),1+OFFSET(U13,0,-1),1+OFFSET(U13,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="V13" s="2" cm="1">
         <f t="array" aca="1" ref="V13" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P13,0),OFFSET(V13,-1,-1),MIN(1+OFFSET(V13,-1,0),1+OFFSET(V13,0,-1),1+OFFSET(V13,-1,-1)))</f>
@@ -1422,11 +1424,11 @@
       </c>
       <c r="W13" s="2" cm="1">
         <f t="array" aca="1" ref="W13" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P13,0),OFFSET(W13,-1,-1),MIN(1+OFFSET(W13,-1,0),1+OFFSET(W13,0,-1),1+OFFSET(W13,-1,-1)))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X13" s="2" cm="1">
         <f t="array" aca="1" ref="X13" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P13,0),OFFSET(X13,-1,-1),MIN(1+OFFSET(X13,-1,0),1+OFFSET(X13,0,-1),1+OFFSET(X13,-1,-1)))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Y13" s="2" cm="1">
         <f t="array" aca="1" ref="Y13" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P13,0),OFFSET(Y13,-1,-1),MIN(1+OFFSET(Y13,-1,0),1+OFFSET(Y13,0,-1),1+OFFSET(Y13,-1,-1)))</f>
@@ -1443,20 +1445,20 @@
       <c r="AB13" s="24"/>
       <c r="AE13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>A</v>
       </c>
       <c r="AF13" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>B</v>
       </c>
       <c r="AG13" s="1">
         <v>6</v>
       </c>
       <c r="AH13" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="13"/>
       <c r="B14" s="13"/>
       <c r="C14" s="13"/>
@@ -1488,53 +1490,53 @@
       </c>
       <c r="T14" s="2" cm="1">
         <f t="array" aca="1" ref="T14" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P14,0),OFFSET(T14,-1,-1),MIN(1+OFFSET(T14,-1,0),1+OFFSET(T14,0,-1),1+OFFSET(T14,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U14" s="2" cm="1">
         <f t="array" aca="1" ref="U14" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P14,0),OFFSET(U14,-1,-1),MIN(1+OFFSET(U14,-1,0),1+OFFSET(U14,0,-1),1+OFFSET(U14,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="V14" s="2" cm="1">
         <f t="array" aca="1" ref="V14" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P14,0),OFFSET(V14,-1,-1),MIN(1+OFFSET(V14,-1,0),1+OFFSET(V14,0,-1),1+OFFSET(V14,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="W14" s="2" cm="1">
         <f t="array" aca="1" ref="W14" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P14,0),OFFSET(W14,-1,-1),MIN(1+OFFSET(W14,-1,0),1+OFFSET(W14,0,-1),1+OFFSET(W14,-1,-1)))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X14" s="2" cm="1">
         <f t="array" aca="1" ref="X14" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P14,0),OFFSET(X14,-1,-1),MIN(1+OFFSET(X14,-1,0),1+OFFSET(X14,0,-1),1+OFFSET(X14,-1,-1)))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Y14" s="2" cm="1">
         <f t="array" aca="1" ref="Y14" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P14,0),OFFSET(Y14,-1,-1),MIN(1+OFFSET(Y14,-1,0),1+OFFSET(Y14,0,-1),1+OFFSET(Y14,-1,-1)))</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="Z14" s="2" cm="1">
         <f t="array" aca="1" ref="Z14" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P14,0),OFFSET(Z14,-1,-1),MIN(1+OFFSET(Z14,-1,0),1+OFFSET(Z14,0,-1),1+OFFSET(Z14,-1,-1)))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AA14" s="2" cm="1">
         <f t="array" aca="1" ref="AA14" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P14,0),OFFSET(AA14,-1,-1),MIN(1+OFFSET(AA14,-1,0),1+OFFSET(AA14,0,-1),1+OFFSET(AA14,-1,-1)))</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AB14" s="24"/>
       <c r="AE14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>T</v>
       </c>
       <c r="AF14" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>E</v>
       </c>
       <c r="AG14" s="1">
         <v>7</v>
       </c>
       <c r="AH14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="13"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1566,56 +1568,56 @@
       </c>
       <c r="T15" s="2" cm="1">
         <f t="array" aca="1" ref="T15" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P15,0),OFFSET(T15,-1,-1),MIN(1+OFFSET(T15,-1,0),1+OFFSET(T15,0,-1),1+OFFSET(T15,-1,-1)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="U15" s="2" cm="1">
         <f t="array" aca="1" ref="U15" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P15,0),OFFSET(U15,-1,-1),MIN(1+OFFSET(U15,-1,0),1+OFFSET(U15,0,-1),1+OFFSET(U15,-1,-1)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="V15" s="2" cm="1">
         <f t="array" aca="1" ref="V15" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P15,0),OFFSET(V15,-1,-1),MIN(1+OFFSET(V15,-1,0),1+OFFSET(V15,0,-1),1+OFFSET(V15,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="W15" s="2" cm="1">
         <f t="array" aca="1" ref="W15" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P15,0),OFFSET(W15,-1,-1),MIN(1+OFFSET(W15,-1,0),1+OFFSET(W15,0,-1),1+OFFSET(W15,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="X15" s="2" cm="1">
         <f t="array" aca="1" ref="X15" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P15,0),OFFSET(X15,-1,-1),MIN(1+OFFSET(X15,-1,0),1+OFFSET(X15,0,-1),1+OFFSET(X15,-1,-1)))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Y15" s="2" cm="1">
         <f t="array" aca="1" ref="Y15" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P15,0),OFFSET(Y15,-1,-1),MIN(1+OFFSET(Y15,-1,0),1+OFFSET(Y15,0,-1),1+OFFSET(Y15,-1,-1)))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Z15" s="2" cm="1">
         <f t="array" aca="1" ref="Z15" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P15,0),OFFSET(Z15,-1,-1),MIN(1+OFFSET(Z15,-1,0),1+OFFSET(Z15,0,-1),1+OFFSET(Z15,-1,-1)))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AA15" s="2" cm="1">
         <f t="array" aca="1" ref="AA15" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P15,0),OFFSET(AA15,-1,-1),MIN(1+OFFSET(AA15,-1,0),1+OFFSET(AA15,0,-1),1+OFFSET(AA15,-1,-1)))</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AB15" s="24"/>
       <c r="AE15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Z</v>
       </c>
       <c r="AF15" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>F</v>
       </c>
       <c r="AG15" s="1">
         <v>8</v>
       </c>
       <c r="AH15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AJ15" s="6"/>
     </row>
-    <row r="16" spans="1:36" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:36" ht="21" customHeight="1" x14ac:dyDescent="0.15">
       <c r="O16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="P16" s="3">
         <v>10</v>
@@ -1633,35 +1635,35 @@
       </c>
       <c r="T16" s="2" cm="1">
         <f t="array" aca="1" ref="T16" ca="1">IF(INDEX(X,T$5,0)=INDEX(Y,$P16,0),OFFSET(T16,-1,-1),MIN(1+OFFSET(T16,-1,0),1+OFFSET(T16,0,-1),1+OFFSET(T16,-1,-1)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="U16" s="2" cm="1">
         <f t="array" aca="1" ref="U16" ca="1">IF(INDEX(X,U$5,0)=INDEX(Y,$P16,0),OFFSET(U16,-1,-1),MIN(1+OFFSET(U16,-1,0),1+OFFSET(U16,0,-1),1+OFFSET(U16,-1,-1)))</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="V16" s="2" cm="1">
         <f t="array" aca="1" ref="V16" ca="1">IF(INDEX(X,V$5,0)=INDEX(Y,$P16,0),OFFSET(V16,-1,-1),MIN(1+OFFSET(V16,-1,0),1+OFFSET(V16,0,-1),1+OFFSET(V16,-1,-1)))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="W16" s="2" cm="1">
         <f t="array" aca="1" ref="W16" ca="1">IF(INDEX(X,W$5,0)=INDEX(Y,$P16,0),OFFSET(W16,-1,-1),MIN(1+OFFSET(W16,-1,0),1+OFFSET(W16,0,-1),1+OFFSET(W16,-1,-1)))</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="X16" s="2" cm="1">
         <f t="array" aca="1" ref="X16" ca="1">IF(INDEX(X,X$5,0)=INDEX(Y,$P16,0),OFFSET(X16,-1,-1),MIN(1+OFFSET(X16,-1,0),1+OFFSET(X16,0,-1),1+OFFSET(X16,-1,-1)))</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Y16" s="2" cm="1">
         <f t="array" aca="1" ref="Y16" ca="1">IF(INDEX(X,Y$5,0)=INDEX(Y,$P16,0),OFFSET(Y16,-1,-1),MIN(1+OFFSET(Y16,-1,0),1+OFFSET(Y16,0,-1),1+OFFSET(Y16,-1,-1)))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z16" s="2" cm="1">
         <f t="array" aca="1" ref="Z16" ca="1">IF(INDEX(X,Z$5,0)=INDEX(Y,$P16,0),OFFSET(Z16,-1,-1),MIN(1+OFFSET(Z16,-1,0),1+OFFSET(Z16,0,-1),1+OFFSET(Z16,-1,-1)))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AA16" s="2" cm="1">
         <f t="array" aca="1" ref="AA16" ca="1">IF(INDEX(X,AA$5,0)=INDEX(Y,$P16,0),OFFSET(AA16,-1,-1),MIN(1+OFFSET(AA16,-1,0),1+OFFSET(AA16,0,-1),1+OFFSET(AA16,-1,-1)))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AB16" s="24"/>
       <c r="AE16" s="7" t="str">
@@ -1670,7 +1672,7 @@
       </c>
       <c r="AF16" s="7" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>A</v>
       </c>
       <c r="AG16" s="1">
         <v>9</v>
@@ -1702,11 +1704,11 @@
       <c r="AD18" s="6"/>
       <c r="AE18" s="8">
         <f>COUNTIFS(AE$7:AE$16,"?")</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="AF18" s="8">
         <f>COUNTIFS(AF$7:AF$16,"?")</f>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AG18" s="11" t="s">
         <v>21</v>
@@ -1717,27 +1719,27 @@
         <v>23</v>
       </c>
       <c r="AF20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG20" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AH20" s="25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="AE21" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AF21" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AF21" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="AG21" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AH21" s="25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1746,13 +1748,13 @@
         <v>PBBCEFATZAF</v>
       </c>
       <c r="AF22" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AG22" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="AH22" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="16:36" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1761,13 +1763,13 @@
         <v>PBBCEFATAF</v>
       </c>
       <c r="AF23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG23" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AG23" s="25" t="s">
-        <v>45</v>
-      </c>
       <c r="AH23" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1775,7 +1777,7 @@
     <mergeCell ref="AE4:AF4"/>
   </mergeCells>
   <conditionalFormatting sqref="Q6:AB16">
-    <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="2" stopIfTrue="1">
       <formula>AND($P6=$AF$18,Q$5=$AE$18)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>